<commit_message>
v0.007 First tests setup (the wrong way)
</commit_message>
<xml_diff>
--- a/FBM-planning.xlsx
+++ b/FBM-planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="37">
   <si>
     <t>M</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>**League ?</t>
+  </si>
+  <si>
+    <t>Testing with xUnit Manning LiveProject</t>
   </si>
 </sst>
 </file>
@@ -732,7 +735,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S11" sqref="S11:T11"/>
+      <selection pane="topRight" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1655,6 +1658,9 @@
       <c r="AC35" s="21"/>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A36" s="22" t="s">
+        <v>36</v>
+      </c>
       <c r="G36" s="21"/>
       <c r="H36" s="21"/>
       <c r="N36" s="21"/>

</xml_diff>

<commit_message>
v0.009 Setup Tests; Manager, Fixtures
</commit_message>
<xml_diff>
--- a/FBM-planning.xlsx
+++ b/FBM-planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="39">
   <si>
     <t>M</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>Testing with xUnit Manning LiveProject</t>
+  </si>
+  <si>
+    <t>Test 1. Calc fixtures</t>
+  </si>
+  <si>
+    <t>Test 2. Calc match results</t>
   </si>
 </sst>
 </file>
@@ -733,9 +739,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A36" sqref="A36"/>
+      <selection pane="topRight" activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,10 +1113,10 @@
       <c r="M11" s="23"/>
       <c r="N11" s="21"/>
       <c r="O11" s="21"/>
-      <c r="S11" s="41"/>
-      <c r="T11" s="41"/>
       <c r="U11" s="21"/>
       <c r="V11" s="21"/>
+      <c r="Y11" s="41"/>
+      <c r="Z11" s="41"/>
       <c r="AB11" s="21"/>
       <c r="AC11" s="21"/>
     </row>
@@ -1131,9 +1137,10 @@
       <c r="N12" s="21"/>
       <c r="O12" s="21"/>
       <c r="R12" s="40"/>
-      <c r="S12" s="41"/>
+      <c r="S12" s="40"/>
       <c r="U12" s="21"/>
       <c r="V12" s="21"/>
+      <c r="W12" s="41"/>
       <c r="AB12" s="21"/>
       <c r="AC12" s="21"/>
     </row>
@@ -1277,10 +1284,10 @@
       <c r="N18" s="34"/>
       <c r="O18" s="34"/>
       <c r="P18" s="33"/>
-      <c r="S18" s="41"/>
-      <c r="T18" s="41"/>
       <c r="U18" s="21"/>
       <c r="V18" s="21"/>
+      <c r="Y18" s="41"/>
+      <c r="Z18" s="41"/>
       <c r="AB18" s="21"/>
       <c r="AC18" s="21"/>
     </row>
@@ -1626,10 +1633,10 @@
       <c r="H33" s="21"/>
       <c r="N33" s="21"/>
       <c r="O33" s="21"/>
-      <c r="S33" s="42"/>
-      <c r="T33" s="42"/>
       <c r="U33" s="21"/>
       <c r="V33" s="21"/>
+      <c r="W33" s="42"/>
+      <c r="X33" s="42"/>
       <c r="AB33" s="21"/>
       <c r="AC33" s="21"/>
     </row>
@@ -1671,6 +1678,9 @@
       <c r="AC36" s="21"/>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>37</v>
+      </c>
       <c r="G37" s="21"/>
       <c r="H37" s="21"/>
       <c r="N37" s="21"/>
@@ -1681,6 +1691,9 @@
       <c r="AC37" s="21"/>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>38</v>
+      </c>
       <c r="G38" s="21"/>
       <c r="H38" s="21"/>
       <c r="N38" s="21"/>

</xml_diff>

<commit_message>
v0.011 Fixing tests 1-6
</commit_message>
<xml_diff>
--- a/FBM-planning.xlsx
+++ b/FBM-planning.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="21075" windowHeight="12345"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="21075" windowHeight="12345" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Feb" sheetId="1" r:id="rId1"/>
     <sheet name="Mars" sheetId="2" r:id="rId2"/>
     <sheet name="April" sheetId="3" r:id="rId3"/>
+    <sheet name="Tests" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="58">
   <si>
     <t>M</t>
   </si>
@@ -126,13 +127,70 @@
     <t>**League ?</t>
   </si>
   <si>
-    <t>Testing with xUnit Manning LiveProject</t>
-  </si>
-  <si>
-    <t>Test 1. Calc fixtures</t>
-  </si>
-  <si>
-    <t>Test 2. Calc match results</t>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Impl. Date</t>
+  </si>
+  <si>
+    <t>Calc fixtures</t>
+  </si>
+  <si>
+    <t>Calc match results</t>
+  </si>
+  <si>
+    <t>UT001</t>
+  </si>
+  <si>
+    <t>UT002</t>
+  </si>
+  <si>
+    <t>UT003</t>
+  </si>
+  <si>
+    <t>UT004</t>
+  </si>
+  <si>
+    <t>UT005</t>
+  </si>
+  <si>
+    <t>UT006</t>
+  </si>
+  <si>
+    <t>UT007</t>
+  </si>
+  <si>
+    <t>UT008</t>
+  </si>
+  <si>
+    <t>UT009</t>
+  </si>
+  <si>
+    <t>UT010</t>
+  </si>
+  <si>
+    <t>Match Draw</t>
+  </si>
+  <si>
+    <t>Match Win</t>
+  </si>
+  <si>
+    <t>Match Lost</t>
+  </si>
+  <si>
+    <t>Goal Home Team</t>
+  </si>
+  <si>
+    <t>Goal Away Team</t>
+  </si>
+  <si>
+    <t>Test/Function</t>
+  </si>
+  <si>
+    <t>Display League table</t>
+  </si>
+  <si>
+    <t>Display Match</t>
   </si>
 </sst>
 </file>
@@ -142,7 +200,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-41D]dd/mmm;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,8 +223,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,6 +314,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -378,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -436,6 +508,24 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,9 +829,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z18" sqref="Z18:AA18"/>
+      <selection pane="topRight" activeCell="A36" sqref="A36:A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1666,9 +1756,6 @@
       <c r="AC35" s="21"/>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="s">
-        <v>36</v>
-      </c>
       <c r="G36" s="21"/>
       <c r="H36" s="21"/>
       <c r="N36" s="21"/>
@@ -1682,9 +1769,6 @@
       <c r="AC36" s="21"/>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
-        <v>37</v>
-      </c>
       <c r="G37" s="21"/>
       <c r="H37" s="21"/>
       <c r="N37" s="21"/>
@@ -1698,9 +1782,6 @@
       <c r="AC37" s="21"/>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
-        <v>38</v>
-      </c>
       <c r="G38" s="21"/>
       <c r="H38" s="21"/>
       <c r="N38" s="21"/>
@@ -2100,4 +2181,217 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="36.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="32" width="7.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="54"/>
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="54"/>
+    </row>
+    <row r="2" spans="1:33" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="52"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
+      <c r="Y2" s="49"/>
+      <c r="Z2" s="49"/>
+      <c r="AA2" s="49"/>
+      <c r="AB2" s="49"/>
+      <c r="AC2" s="49"/>
+      <c r="AD2" s="49"/>
+      <c r="AE2" s="49"/>
+      <c r="AF2" s="49"/>
+      <c r="AG2" s="50"/>
+    </row>
+    <row r="3" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="22"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="39"/>
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="39"/>
+      <c r="AD3" s="39"/>
+      <c r="AE3" s="39"/>
+      <c r="AF3" s="39"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="57" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="58" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="58" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="58" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="56">
+        <v>44615</v>
+      </c>
+      <c r="D9" s="38"/>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="56">
+        <v>44615</v>
+      </c>
+      <c r="D10" s="38"/>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
v0.012 Create Manager and Choosing Team
</commit_message>
<xml_diff>
--- a/FBM-planning.xlsx
+++ b/FBM-planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="21075" windowHeight="12345" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="21075" windowHeight="12345" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feb" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="58">
   <si>
     <t>M</t>
   </si>
@@ -829,9 +829,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD38"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A36" sqref="A36:A38"/>
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A11" sqref="A11:A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,8 +1205,6 @@
       <c r="O11" s="21"/>
       <c r="U11" s="21"/>
       <c r="V11" s="21"/>
-      <c r="Z11" s="41"/>
-      <c r="AA11" s="41"/>
       <c r="AB11" s="21"/>
       <c r="AC11" s="21"/>
     </row>
@@ -1230,10 +1228,9 @@
       <c r="S12" s="40"/>
       <c r="U12" s="21"/>
       <c r="V12" s="21"/>
-      <c r="W12" s="41"/>
-      <c r="X12" s="41"/>
       <c r="AB12" s="21"/>
       <c r="AC12" s="21"/>
+      <c r="AD12" s="41"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
@@ -1377,8 +1374,6 @@
       <c r="P18" s="33"/>
       <c r="U18" s="21"/>
       <c r="V18" s="21"/>
-      <c r="Z18" s="41"/>
-      <c r="AA18" s="41"/>
       <c r="AB18" s="21"/>
       <c r="AC18" s="21"/>
     </row>
@@ -1632,10 +1627,6 @@
       <c r="U27" s="27"/>
       <c r="V27" s="27"/>
       <c r="W27" s="26"/>
-      <c r="X27" s="26"/>
-      <c r="Y27" s="26"/>
-      <c r="Z27" s="26"/>
-      <c r="AA27" s="28"/>
       <c r="AB27" s="21"/>
       <c r="AC27" s="21"/>
     </row>
@@ -1650,9 +1641,6 @@
       <c r="Q28" s="23"/>
       <c r="U28" s="21"/>
       <c r="V28" s="21"/>
-      <c r="Y28" s="42"/>
-      <c r="Z28" s="42"/>
-      <c r="AA28" s="42"/>
       <c r="AB28" s="21"/>
       <c r="AC28" s="21"/>
     </row>
@@ -1667,8 +1655,6 @@
       <c r="U29" s="21"/>
       <c r="V29" s="21"/>
       <c r="W29" s="23"/>
-      <c r="Y29" s="42"/>
-      <c r="Z29" s="42"/>
       <c r="AB29" s="21"/>
       <c r="AC29" s="21"/>
     </row>
@@ -1683,8 +1669,6 @@
       <c r="U30" s="21"/>
       <c r="V30" s="21"/>
       <c r="W30" s="23"/>
-      <c r="Y30" s="42"/>
-      <c r="Z30" s="42"/>
       <c r="AB30" s="21"/>
       <c r="AC30" s="21"/>
     </row>
@@ -1698,7 +1682,6 @@
       <c r="O31" s="21"/>
       <c r="U31" s="21"/>
       <c r="V31" s="21"/>
-      <c r="AA31" s="42"/>
       <c r="AB31" s="21"/>
       <c r="AC31" s="21"/>
     </row>
@@ -1712,11 +1695,10 @@
       <c r="O32" s="21"/>
       <c r="U32" s="21"/>
       <c r="V32" s="21"/>
-      <c r="AA32" s="42"/>
       <c r="AB32" s="21"/>
       <c r="AC32" s="21"/>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33" s="30" t="s">
         <v>31</v>
       </c>
@@ -1726,12 +1708,11 @@
       <c r="O33" s="21"/>
       <c r="U33" s="21"/>
       <c r="V33" s="21"/>
-      <c r="W33" s="42"/>
-      <c r="X33" s="42"/>
       <c r="AB33" s="21"/>
       <c r="AC33" s="21"/>
-    </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD33" s="42"/>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
       <c r="G34" s="21"/>
       <c r="H34" s="21"/>
@@ -1742,7 +1723,7 @@
       <c r="AB34" s="21"/>
       <c r="AC34" s="21"/>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>32</v>
       </c>
@@ -1755,33 +1736,29 @@
       <c r="AB35" s="21"/>
       <c r="AC35" s="21"/>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
       <c r="G36" s="21"/>
       <c r="H36" s="21"/>
       <c r="N36" s="21"/>
       <c r="O36" s="21"/>
       <c r="U36" s="21"/>
       <c r="V36" s="21"/>
-      <c r="W36" s="42"/>
-      <c r="X36" s="42"/>
-      <c r="Y36" s="42"/>
       <c r="AB36" s="21"/>
       <c r="AC36" s="21"/>
-    </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD36" s="42"/>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="G37" s="21"/>
       <c r="H37" s="21"/>
       <c r="N37" s="21"/>
       <c r="O37" s="21"/>
       <c r="U37" s="21"/>
       <c r="V37" s="21"/>
-      <c r="W37" s="42"/>
-      <c r="X37" s="42"/>
-      <c r="Y37" s="42"/>
       <c r="AB37" s="21"/>
       <c r="AC37" s="21"/>
-    </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD37" s="42"/>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="G38" s="21"/>
       <c r="H38" s="21"/>
       <c r="N38" s="21"/>
@@ -1799,10 +1776,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AF3"/>
+  <dimension ref="A2:AF30"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AC3" sqref="AC3:AF3"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1986,6 +1963,154 @@
       <c r="AF3" s="4" t="s">
         <v>1</v>
       </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="41"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" s="22"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13" s="46" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" s="46" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15" s="46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A16" s="46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="46" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="46" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="28"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="42"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="42"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="42"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="22"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2187,7 +2312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
v0.013 Create New Manager and Choose Team saves to DB
</commit_message>
<xml_diff>
--- a/FBM-planning.xlsx
+++ b/FBM-planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="21075" windowHeight="12345" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="21075" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="Feb" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="59">
   <si>
     <t>M</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>Display Match</t>
+  </si>
+  <si>
+    <t>* Start game (Create Manager, Choose Team)</t>
   </si>
 </sst>
 </file>
@@ -232,7 +235,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +323,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -526,6 +535,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -829,14 +839,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A11" sqref="A11:A35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="30" width="6.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1632,7 +1642,7 @@
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="G28" s="21"/>
       <c r="H28" s="21"/>
@@ -1641,6 +1651,7 @@
       <c r="Q28" s="23"/>
       <c r="U28" s="21"/>
       <c r="V28" s="21"/>
+      <c r="W28" s="59"/>
       <c r="AB28" s="21"/>
       <c r="AC28" s="21"/>
     </row>
@@ -1778,7 +1789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AF30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
v0.014 Manager CRU works, D still to be done.
</commit_message>
<xml_diff>
--- a/FBM-planning.xlsx
+++ b/FBM-planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="21075" windowHeight="12345"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="21075" windowHeight="12345" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feb" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="58">
   <si>
     <t>M</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>Game Functions</t>
-  </si>
-  <si>
-    <t>* Start game</t>
   </si>
   <si>
     <t>* Play through game</t>
@@ -235,7 +232,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,12 +320,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -535,7 +526,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -839,9 +830,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B8" sqref="B8"/>
+      <selection pane="topRight" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,35 +1018,35 @@
       <c r="N3" s="21"/>
       <c r="O3" s="21"/>
       <c r="R3" s="48" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S3" s="43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="T3" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U3" s="21"/>
       <c r="V3" s="21"/>
       <c r="W3" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="X3" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y3" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Z3" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AA3" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AB3" s="21"/>
       <c r="AC3" s="21"/>
       <c r="AD3" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
@@ -1136,7 +1127,7 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
@@ -1157,7 +1148,7 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
@@ -1178,7 +1169,7 @@
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
@@ -1199,7 +1190,7 @@
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
@@ -1220,7 +1211,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -1263,7 +1254,7 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="33"/>
@@ -1365,7 +1356,7 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" s="32"/>
       <c r="C18" s="33"/>
@@ -1389,7 +1380,7 @@
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="32"/>
       <c r="C19" s="33"/>
@@ -1642,7 +1633,7 @@
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G28" s="21"/>
       <c r="H28" s="21"/>
@@ -1651,13 +1642,13 @@
       <c r="Q28" s="23"/>
       <c r="U28" s="21"/>
       <c r="V28" s="21"/>
-      <c r="W28" s="59"/>
+      <c r="W28" s="38"/>
       <c r="AB28" s="21"/>
       <c r="AC28" s="21"/>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G29" s="21"/>
       <c r="H29" s="21"/>
@@ -1671,7 +1662,7 @@
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
@@ -1685,7 +1676,7 @@
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G31" s="21"/>
       <c r="H31" s="21"/>
@@ -1698,7 +1689,7 @@
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G32" s="21"/>
       <c r="H32" s="21"/>
@@ -1711,7 +1702,7 @@
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G33" s="21"/>
       <c r="H33" s="21"/>
@@ -1736,7 +1727,7 @@
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G35" s="21"/>
       <c r="H35" s="21"/>
@@ -1789,13 +1780,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AF30"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.140625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="41.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="32" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1977,23 +1968,24 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="41"/>
       <c r="E4" s="41"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="41"/>
+        <v>29</v>
+      </c>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
@@ -2013,14 +2005,14 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="41"/>
       <c r="E11" s="41"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
@@ -2043,85 +2035,93 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="46" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="47" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="31" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
-      <c r="E20" s="28"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="28"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
+      <c r="E22" s="42"/>
+      <c r="H22" s="42"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="42"/>
+      <c r="H23" s="42"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="42"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I24" s="42"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="42"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I25" s="42"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="42"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="22"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="42"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="42"/>
-      <c r="C29" s="42"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J29" s="42"/>
+      <c r="K29" s="42"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J30" s="42"/>
+      <c r="K30" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2337,13 +2337,13 @@
   <sheetData>
     <row r="1" spans="1:33" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" s="53" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D1" s="54" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="54"/>
       <c r="F1" s="54"/>
@@ -2443,50 +2443,50 @@
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="57" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="58" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="58" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="58" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="56">
         <v>44615</v>
@@ -2495,10 +2495,10 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="56">
         <v>44615</v>
@@ -2507,23 +2507,23 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v0.017 Choose Manager + Team + Create Fixtures
</commit_message>
<xml_diff>
--- a/FBM-planning.xlsx
+++ b/FBM-planning.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="59">
   <si>
     <t>M</t>
   </si>
@@ -94,9 +94,6 @@
     <t>**Fixtures</t>
   </si>
   <si>
-    <t>Create/Read Manager</t>
-  </si>
-  <si>
     <t>Create/Read Team</t>
   </si>
   <si>
@@ -191,6 +188,12 @@
   </si>
   <si>
     <t>* Start game (Create Manager, Choose Team)</t>
+  </si>
+  <si>
+    <t>Create/Read Manager/Update</t>
+  </si>
+  <si>
+    <t>Create/Read/Update Fixtures</t>
   </si>
 </sst>
 </file>
@@ -232,7 +235,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +323,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -484,7 +493,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -527,6 +535,7 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -832,7 +841,7 @@
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A28" sqref="A28"/>
+      <selection pane="topRight" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,46 +1026,46 @@
       <c r="M3" s="21"/>
       <c r="N3" s="21"/>
       <c r="O3" s="21"/>
-      <c r="R3" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="S3" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="T3" s="44" t="s">
-        <v>33</v>
+      <c r="R3" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="43" t="s">
+        <v>32</v>
       </c>
       <c r="U3" s="21"/>
       <c r="V3" s="21"/>
-      <c r="W3" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="X3" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y3" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z3" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA3" s="44" t="s">
-        <v>33</v>
+      <c r="W3" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="X3" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y3" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z3" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA3" s="43" t="s">
+        <v>32</v>
       </c>
       <c r="AB3" s="21"/>
       <c r="AC3" s="21"/>
-      <c r="AD3" s="44" t="s">
-        <v>33</v>
+      <c r="AD3" s="43" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
       <c r="G4" s="21"/>
       <c r="H4" s="21"/>
       <c r="N4" s="21"/>
@@ -1071,10 +1080,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="23"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
       <c r="N5" s="21"/>
@@ -1089,10 +1098,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="23"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
       <c r="N6" s="21"/>
@@ -1103,21 +1112,21 @@
       <c r="AC6" s="21"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
       <c r="N7" s="21"/>
       <c r="O7" s="21"/>
       <c r="U7" s="21"/>
@@ -1126,8 +1135,8 @@
       <c r="AC7" s="21"/>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>25</v>
+      <c r="A8" s="45" t="s">
+        <v>57</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
@@ -1138,7 +1147,7 @@
       <c r="J8" s="23"/>
       <c r="K8" s="23"/>
       <c r="L8" s="23"/>
-      <c r="M8" s="38"/>
+      <c r="M8" s="37"/>
       <c r="N8" s="21"/>
       <c r="O8" s="21"/>
       <c r="U8" s="21"/>
@@ -1147,8 +1156,8 @@
       <c r="AC8" s="21"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>26</v>
+      <c r="A9" s="45" t="s">
+        <v>25</v>
       </c>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
@@ -1158,8 +1167,8 @@
       <c r="I9" s="23"/>
       <c r="J9" s="23"/>
       <c r="K9" s="23"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
       <c r="N9" s="21"/>
       <c r="O9" s="21"/>
       <c r="U9" s="21"/>
@@ -1168,8 +1177,8 @@
       <c r="AC9" s="21"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>27</v>
+      <c r="A10" s="45" t="s">
+        <v>26</v>
       </c>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
@@ -1178,7 +1187,7 @@
       <c r="H10" s="21"/>
       <c r="I10" s="23"/>
       <c r="J10" s="23"/>
-      <c r="K10" s="38"/>
+      <c r="K10" s="37"/>
       <c r="L10" s="23"/>
       <c r="M10" s="23"/>
       <c r="N10" s="21"/>
@@ -1190,7 +1199,7 @@
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
@@ -1210,8 +1219,8 @@
       <c r="AC11" s="21"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>29</v>
+      <c r="A12" s="45" t="s">
+        <v>28</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -1220,18 +1229,18 @@
       <c r="H12" s="21"/>
       <c r="I12" s="23"/>
       <c r="J12" s="23"/>
-      <c r="K12" s="38"/>
+      <c r="K12" s="37"/>
       <c r="L12" s="23"/>
       <c r="M12" s="23"/>
       <c r="N12" s="21"/>
       <c r="O12" s="21"/>
-      <c r="R12" s="40"/>
-      <c r="S12" s="40"/>
+      <c r="R12" s="39"/>
+      <c r="S12" s="39"/>
       <c r="U12" s="21"/>
       <c r="V12" s="21"/>
       <c r="AB12" s="21"/>
       <c r="AC12" s="21"/>
-      <c r="AD12" s="41"/>
+      <c r="AD12" s="40"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
@@ -1256,11 +1265,11 @@
       <c r="A14" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
       <c r="N14" s="21"/>
@@ -1271,328 +1280,328 @@
       <c r="AC14" s="21"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
-      <c r="P15" s="33"/>
-      <c r="Q15" s="33"/>
-      <c r="R15" s="33"/>
-      <c r="S15" s="33"/>
-      <c r="T15" s="33"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="33"/>
+      <c r="O15" s="33"/>
+      <c r="P15" s="32"/>
+      <c r="Q15" s="32"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="32"/>
+      <c r="T15" s="32"/>
       <c r="U15" s="21"/>
       <c r="V15" s="21"/>
       <c r="AB15" s="21"/>
       <c r="AC15" s="21"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="34"/>
-      <c r="P16" s="33"/>
-      <c r="Q16" s="33"/>
-      <c r="R16" s="33"/>
-      <c r="S16" s="33"/>
-      <c r="T16" s="33"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="33"/>
+      <c r="O16" s="33"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="32"/>
+      <c r="T16" s="32"/>
       <c r="U16" s="21"/>
       <c r="V16" s="21"/>
       <c r="AB16" s="21"/>
       <c r="AC16" s="21"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="34"/>
-      <c r="P17" s="33"/>
-      <c r="Q17" s="33"/>
-      <c r="R17" s="33"/>
-      <c r="S17" s="33"/>
-      <c r="T17" s="33"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="33"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="32"/>
+      <c r="T17" s="32"/>
       <c r="U17" s="21"/>
       <c r="V17" s="21"/>
       <c r="AB17" s="21"/>
       <c r="AC17" s="21"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
-      <c r="N18" s="34"/>
-      <c r="O18" s="34"/>
-      <c r="P18" s="33"/>
+      <c r="A18" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="31"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="33"/>
+      <c r="P18" s="32"/>
       <c r="U18" s="21"/>
       <c r="V18" s="21"/>
       <c r="AB18" s="21"/>
       <c r="AC18" s="21"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="34"/>
-      <c r="P19" s="33"/>
-      <c r="Q19" s="40"/>
-      <c r="R19" s="40"/>
-      <c r="S19" s="33"/>
-      <c r="T19" s="33"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="33"/>
+      <c r="O19" s="33"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="39"/>
+      <c r="R19" s="39"/>
+      <c r="S19" s="32"/>
+      <c r="T19" s="32"/>
       <c r="U19" s="21"/>
       <c r="V19" s="21"/>
       <c r="AB19" s="21"/>
       <c r="AC19" s="21"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="33"/>
-      <c r="Q20" s="33"/>
-      <c r="R20" s="33"/>
-      <c r="S20" s="33"/>
-      <c r="T20" s="33"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="33"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="32"/>
+      <c r="R20" s="32"/>
+      <c r="S20" s="32"/>
+      <c r="T20" s="32"/>
       <c r="U20" s="21"/>
       <c r="V20" s="21"/>
       <c r="AB20" s="21"/>
       <c r="AC20" s="21"/>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="34"/>
-      <c r="P21" s="33"/>
-      <c r="Q21" s="33"/>
-      <c r="R21" s="33"/>
-      <c r="S21" s="33"/>
-      <c r="T21" s="33"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="33"/>
+      <c r="O21" s="33"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="32"/>
+      <c r="R21" s="32"/>
+      <c r="S21" s="32"/>
+      <c r="T21" s="32"/>
       <c r="U21" s="21"/>
       <c r="V21" s="21"/>
       <c r="AB21" s="21"/>
       <c r="AC21" s="21"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A22" s="46" t="s">
+      <c r="A22" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="34"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="33"/>
-      <c r="R22" s="33"/>
-      <c r="S22" s="33"/>
-      <c r="T22" s="33"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="33"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="32"/>
+      <c r="Q22" s="32"/>
+      <c r="R22" s="32"/>
+      <c r="S22" s="32"/>
+      <c r="T22" s="32"/>
       <c r="U22" s="21"/>
       <c r="V22" s="21"/>
       <c r="AB22" s="21"/>
       <c r="AC22" s="21"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="34"/>
-      <c r="O23" s="34"/>
-      <c r="P23" s="33"/>
-      <c r="Q23" s="33"/>
-      <c r="R23" s="33"/>
-      <c r="S23" s="33"/>
-      <c r="T23" s="33"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="33"/>
+      <c r="O23" s="33"/>
+      <c r="P23" s="32"/>
+      <c r="Q23" s="32"/>
+      <c r="R23" s="32"/>
+      <c r="S23" s="32"/>
+      <c r="T23" s="32"/>
       <c r="U23" s="21"/>
       <c r="V23" s="21"/>
       <c r="AB23" s="21"/>
       <c r="AC23" s="21"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="32"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="38"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="34"/>
-      <c r="P24" s="33"/>
-      <c r="Q24" s="33"/>
-      <c r="R24" s="33"/>
-      <c r="S24" s="33"/>
-      <c r="T24" s="33"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="33"/>
+      <c r="O24" s="33"/>
+      <c r="P24" s="32"/>
+      <c r="Q24" s="32"/>
+      <c r="R24" s="32"/>
+      <c r="S24" s="32"/>
+      <c r="T24" s="32"/>
       <c r="U24" s="21"/>
       <c r="V24" s="21"/>
       <c r="AB24" s="21"/>
       <c r="AC24" s="21"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="33"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="34"/>
-      <c r="O25" s="34"/>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="33"/>
-      <c r="R25" s="33"/>
-      <c r="S25" s="33"/>
-      <c r="T25" s="33"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="33"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="32"/>
+      <c r="R25" s="32"/>
+      <c r="S25" s="32"/>
+      <c r="T25" s="32"/>
       <c r="U25" s="21"/>
       <c r="V25" s="21"/>
       <c r="AB25" s="21"/>
       <c r="AC25" s="21"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A26" s="47" t="s">
+      <c r="A26" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="35"/>
+      <c r="B26" s="34"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
-      <c r="N26" s="36"/>
-      <c r="O26" s="36"/>
-      <c r="P26" s="38"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="35"/>
+      <c r="P26" s="37"/>
       <c r="Q26" s="7"/>
       <c r="R26" s="7"/>
       <c r="S26" s="7"/>
@@ -1603,37 +1612,37 @@
       <c r="AC26" s="21"/>
     </row>
     <row r="27" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="27"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="26"/>
-      <c r="Q27" s="26"/>
-      <c r="R27" s="26"/>
-      <c r="S27" s="26"/>
-      <c r="T27" s="26"/>
-      <c r="U27" s="27"/>
-      <c r="V27" s="27"/>
-      <c r="W27" s="26"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="25"/>
+      <c r="N27" s="26"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="25"/>
+      <c r="Q27" s="25"/>
+      <c r="R27" s="25"/>
+      <c r="S27" s="25"/>
+      <c r="T27" s="25"/>
+      <c r="U27" s="26"/>
+      <c r="V27" s="26"/>
+      <c r="W27" s="25"/>
       <c r="AB27" s="21"/>
       <c r="AC27" s="21"/>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A28" s="29" t="s">
-        <v>57</v>
+      <c r="A28" s="28" t="s">
+        <v>56</v>
       </c>
       <c r="G28" s="21"/>
       <c r="H28" s="21"/>
@@ -1642,12 +1651,12 @@
       <c r="Q28" s="23"/>
       <c r="U28" s="21"/>
       <c r="V28" s="21"/>
-      <c r="W28" s="38"/>
+      <c r="W28" s="37"/>
       <c r="AB28" s="21"/>
       <c r="AC28" s="21"/>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="29" t="s">
         <v>20</v>
       </c>
       <c r="G29" s="21"/>
@@ -1661,7 +1670,7 @@
       <c r="AC29" s="21"/>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="29" t="s">
         <v>22</v>
       </c>
       <c r="G30" s="21"/>
@@ -1675,7 +1684,7 @@
       <c r="AC30" s="21"/>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
+      <c r="A31" s="29" t="s">
         <v>21</v>
       </c>
       <c r="G31" s="21"/>
@@ -1688,8 +1697,8 @@
       <c r="AC31" s="21"/>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
-        <v>32</v>
+      <c r="A32" s="29" t="s">
+        <v>31</v>
       </c>
       <c r="G32" s="21"/>
       <c r="H32" s="21"/>
@@ -1701,8 +1710,8 @@
       <c r="AC32" s="21"/>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A33" s="30" t="s">
-        <v>30</v>
+      <c r="A33" s="29" t="s">
+        <v>29</v>
       </c>
       <c r="G33" s="21"/>
       <c r="H33" s="21"/>
@@ -1712,7 +1721,7 @@
       <c r="V33" s="21"/>
       <c r="AB33" s="21"/>
       <c r="AC33" s="21"/>
-      <c r="AD33" s="42"/>
+      <c r="AD33" s="41"/>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
@@ -1727,7 +1736,7 @@
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G35" s="21"/>
       <c r="H35" s="21"/>
@@ -1747,7 +1756,7 @@
       <c r="V36" s="21"/>
       <c r="AB36" s="21"/>
       <c r="AC36" s="21"/>
-      <c r="AD36" s="42"/>
+      <c r="AD36" s="41"/>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="G37" s="21"/>
@@ -1758,7 +1767,7 @@
       <c r="V37" s="21"/>
       <c r="AB37" s="21"/>
       <c r="AC37" s="21"/>
-      <c r="AD37" s="42"/>
+      <c r="AD37" s="41"/>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="G38" s="21"/>
@@ -1781,7 +1790,7 @@
   <dimension ref="A2:AF30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1968,17 +1977,17 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
+        <v>27</v>
+      </c>
+      <c r="E4" s="40"/>
+      <c r="H4" s="40"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
+      <c r="A5" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="39"/>
+      <c r="E5" s="40"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
@@ -1989,139 +1998,140 @@
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="58" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="45" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="45" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
+      <c r="A11" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="45" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="45" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="45" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="45" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="45" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="45" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="45" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="46" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="28"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="27"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
+      <c r="A21" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="42"/>
-      <c r="H22" s="42"/>
+      <c r="E22" s="41"/>
+      <c r="H22" s="41"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="42"/>
-      <c r="H23" s="42"/>
+      <c r="E23" s="41"/>
+      <c r="H23" s="41"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="I24" s="42"/>
+      <c r="I24" s="41"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="I25" s="42"/>
+      <c r="A25" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" s="41"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="42"/>
+      <c r="A26" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="37"/>
+      <c r="E26" s="41"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J29" s="42"/>
-      <c r="K29" s="42"/>
+      <c r="J29" s="41"/>
+      <c r="K29" s="41"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J30" s="42"/>
-      <c r="K30" s="42"/>
+      <c r="J30" s="41"/>
+      <c r="K30" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2335,195 +2345,195 @@
     <col min="33" max="33" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-    </row>
-    <row r="2" spans="1:33" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="52"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="49"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="49"/>
-      <c r="W2" s="49"/>
-      <c r="X2" s="49"/>
-      <c r="Y2" s="49"/>
-      <c r="Z2" s="49"/>
-      <c r="AA2" s="49"/>
-      <c r="AB2" s="49"/>
-      <c r="AC2" s="49"/>
-      <c r="AD2" s="49"/>
-      <c r="AE2" s="49"/>
-      <c r="AF2" s="49"/>
-      <c r="AG2" s="50"/>
-    </row>
-    <row r="3" spans="1:33" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="53"/>
+      <c r="AA1" s="53"/>
+      <c r="AB1" s="53"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="53"/>
+      <c r="AF1" s="53"/>
+    </row>
+    <row r="2" spans="1:33" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="51"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="48"/>
+      <c r="V2" s="48"/>
+      <c r="W2" s="48"/>
+      <c r="X2" s="48"/>
+      <c r="Y2" s="48"/>
+      <c r="Z2" s="48"/>
+      <c r="AA2" s="48"/>
+      <c r="AB2" s="48"/>
+      <c r="AC2" s="48"/>
+      <c r="AD2" s="48"/>
+      <c r="AE2" s="48"/>
+      <c r="AF2" s="48"/>
+      <c r="AG2" s="49"/>
+    </row>
+    <row r="3" spans="1:33" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="22"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="39"/>
-      <c r="W3" s="39"/>
-      <c r="X3" s="39"/>
-      <c r="Y3" s="39"/>
-      <c r="Z3" s="39"/>
-      <c r="AA3" s="39"/>
-      <c r="AB3" s="39"/>
-      <c r="AC3" s="39"/>
-      <c r="AD3" s="39"/>
-      <c r="AE3" s="39"/>
-      <c r="AF3" s="39"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
+      <c r="V3" s="38"/>
+      <c r="W3" s="38"/>
+      <c r="X3" s="38"/>
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="38"/>
+      <c r="AB3" s="38"/>
+      <c r="AC3" s="38"/>
+      <c r="AD3" s="38"/>
+      <c r="AE3" s="38"/>
+      <c r="AF3" s="38"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="57" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="B5" s="56" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="58" t="s">
-        <v>50</v>
+        <v>40</v>
+      </c>
+      <c r="B6" s="57" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="58" t="s">
-        <v>49</v>
+        <v>41</v>
+      </c>
+      <c r="B7" s="57" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="58" t="s">
-        <v>51</v>
+        <v>42</v>
+      </c>
+      <c r="B8" s="57" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="56">
+        <v>51</v>
+      </c>
+      <c r="C9" s="55">
         <v>44615</v>
       </c>
-      <c r="D9" s="38"/>
+      <c r="D9" s="37"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="56">
+        <v>52</v>
+      </c>
+      <c r="C10" s="55">
         <v>44615</v>
       </c>
-      <c r="D10" s="38"/>
+      <c r="D10" s="37"/>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v0.018 Fixed + refactored InitManager, InitFixtures
</commit_message>
<xml_diff>
--- a/FBM-planning.xlsx
+++ b/FBM-planning.xlsx
@@ -1790,7 +1790,7 @@
   <dimension ref="A2:AF30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="H11" sqref="H11:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1979,15 +1979,15 @@
       <c r="A4" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="40"/>
       <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
         <v>58</v>
       </c>
       <c r="D5" s="39"/>
-      <c r="E5" s="40"/>
+      <c r="E5" s="39"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
@@ -2016,8 +2016,8 @@
       <c r="A11" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
@@ -2088,34 +2088,36 @@
       <c r="A22" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="41"/>
       <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="41"/>
       <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
         <v>21</v>
       </c>
       <c r="I24" s="41"/>
+      <c r="J24" s="41"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
         <v>31</v>
       </c>
       <c r="I25" s="41"/>
+      <c r="J25" s="41"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
         <v>29</v>
       </c>
       <c r="D26" s="37"/>
-      <c r="E26" s="41"/>
+      <c r="E26" s="37"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>

</xml_diff>

<commit_message>
v0.022 Fixed Menu flow, List Managed Team Players in GameDay
</commit_message>
<xml_diff>
--- a/FBM-planning.xlsx
+++ b/FBM-planning.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="21075" windowHeight="12345" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="21075" windowHeight="12345" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Feb" sheetId="1" r:id="rId1"/>
     <sheet name="Mars" sheetId="2" r:id="rId2"/>
     <sheet name="April" sheetId="3" r:id="rId3"/>
     <sheet name="Tests" sheetId="5" r:id="rId4"/>
+    <sheet name="Blad1" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="77">
   <si>
     <t>M</t>
   </si>
@@ -194,14 +195,69 @@
   </si>
   <si>
     <t>Create/Read/Update Fixtures</t>
+  </si>
+  <si>
+    <t>Show Main Menu</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Tidrapport</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Slut</t>
+  </si>
+  <si>
+    <t>Uppgift</t>
+  </si>
+  <si>
+    <t>Längd</t>
+  </si>
+  <si>
+    <t>Utbildning Agil projektledning</t>
+  </si>
+  <si>
+    <t>Jobbsök/Uppföljning - Agio</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Excelfix tidrapport</t>
+  </si>
+  <si>
+    <t>LinkedIn, Github fix</t>
+  </si>
+  <si>
+    <t>Lunch</t>
+  </si>
+  <si>
+    <t>Nyheter, C#</t>
+  </si>
+  <si>
+    <t>Paus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-41D]dd/mmm;@"/>
+    <numFmt numFmtId="168" formatCode="hh:mm;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -235,7 +291,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -332,8 +388,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -455,11 +517,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -536,6 +609,14 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="17" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -837,271 +918,296 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD38"/>
+  <dimension ref="A1:AF40"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A12" sqref="A12"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AB1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AF1" sqref="AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="30" width="6.42578125" customWidth="1"/>
+    <col min="32" max="32" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20"/>
-      <c r="B1" s="10">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1">
+        <v>8</v>
+      </c>
+      <c r="C1">
+        <v>8</v>
+      </c>
+      <c r="D1">
+        <v>8</v>
+      </c>
+      <c r="E1">
+        <v>8</v>
+      </c>
+      <c r="F1">
+        <v>8</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>8</v>
+      </c>
+      <c r="L1">
+        <v>8</v>
+      </c>
+      <c r="M1">
+        <v>8</v>
+      </c>
+      <c r="P1">
+        <v>8</v>
+      </c>
+      <c r="Q1">
+        <v>8</v>
+      </c>
+      <c r="R1">
+        <v>8</v>
+      </c>
+      <c r="S1">
+        <v>8</v>
+      </c>
+      <c r="T1">
+        <v>8</v>
+      </c>
+      <c r="W1">
+        <v>8</v>
+      </c>
+      <c r="AD1">
+        <v>8</v>
+      </c>
+      <c r="AF1">
+        <f>SUM(B1:AD1)</f>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="10">
         <v>44592</v>
       </c>
-      <c r="C1" s="10">
+      <c r="C3" s="10">
         <v>44593</v>
       </c>
-      <c r="D1" s="10">
+      <c r="D3" s="10">
         <v>44594</v>
       </c>
-      <c r="E1" s="10">
+      <c r="E3" s="10">
         <v>44595</v>
       </c>
-      <c r="F1" s="10">
+      <c r="F3" s="10">
         <v>44596</v>
       </c>
-      <c r="G1" s="10">
+      <c r="G3" s="10">
         <v>44597</v>
       </c>
-      <c r="H1" s="10">
+      <c r="H3" s="10">
         <v>44598</v>
       </c>
-      <c r="I1" s="10">
+      <c r="I3" s="10">
         <v>44599</v>
       </c>
-      <c r="J1" s="10">
+      <c r="J3" s="10">
         <v>44600</v>
       </c>
-      <c r="K1" s="10">
+      <c r="K3" s="10">
         <v>44601</v>
       </c>
-      <c r="L1" s="10">
+      <c r="L3" s="10">
         <v>44602</v>
       </c>
-      <c r="M1" s="10">
+      <c r="M3" s="10">
         <v>44603</v>
       </c>
-      <c r="N1" s="10">
+      <c r="N3" s="10">
         <v>44604</v>
       </c>
-      <c r="O1" s="10">
+      <c r="O3" s="10">
         <v>44605</v>
       </c>
-      <c r="P1" s="10">
+      <c r="P3" s="10">
         <v>44606</v>
       </c>
-      <c r="Q1" s="10">
+      <c r="Q3" s="10">
         <v>44607</v>
       </c>
-      <c r="R1" s="10">
+      <c r="R3" s="10">
         <v>44608</v>
       </c>
-      <c r="S1" s="10">
+      <c r="S3" s="10">
         <v>44609</v>
       </c>
-      <c r="T1" s="10">
+      <c r="T3" s="10">
         <v>44610</v>
       </c>
-      <c r="U1" s="10">
+      <c r="U3" s="10">
         <v>44611</v>
       </c>
-      <c r="V1" s="10">
+      <c r="V3" s="10">
         <v>44612</v>
       </c>
-      <c r="W1" s="10">
+      <c r="W3" s="10">
         <v>44613</v>
       </c>
-      <c r="X1" s="10">
+      <c r="X3" s="10">
         <v>44614</v>
       </c>
-      <c r="Y1" s="10">
+      <c r="Y3" s="10">
         <v>44615</v>
       </c>
-      <c r="Z1" s="10">
+      <c r="Z3" s="10">
         <v>44616</v>
       </c>
-      <c r="AA1" s="10">
+      <c r="AA3" s="10">
         <v>44617</v>
       </c>
-      <c r="AB1" s="10">
+      <c r="AB3" s="10">
         <v>44618</v>
       </c>
-      <c r="AC1" s="10">
+      <c r="AC3" s="10">
         <v>44619</v>
       </c>
-      <c r="AD1" s="10">
+      <c r="AD3" s="10">
         <v>44620</v>
       </c>
     </row>
-    <row r="2" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13" t="s">
+    <row r="4" spans="1:32" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="13" t="s">
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="13" t="s">
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="14" t="s">
+      <c r="Q4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="15" t="s">
+      <c r="R4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="S4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="T2" s="17" t="s">
+      <c r="T4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="13" t="s">
+      <c r="U4" s="18"/>
+      <c r="V4" s="18"/>
+      <c r="W4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="X2" s="14" t="s">
+      <c r="X4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="Y2" s="15" t="s">
+      <c r="Y4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z2" s="16" t="s">
+      <c r="Z4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="AA2" s="17" t="s">
+      <c r="AA4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="18"/>
-      <c r="AC2" s="18"/>
-      <c r="AD2" s="13" t="s">
+      <c r="AB4" s="18"/>
+      <c r="AC4" s="18"/>
+      <c r="AD4" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="R3" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="S3" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="T3" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="X3" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y3" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z3" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA3" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB3" s="21"/>
-      <c r="AC3" s="21"/>
-      <c r="AD3" s="43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="21"/>
-      <c r="AB4" s="21"/>
-      <c r="AC4" s="21"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
+      <c r="M5" s="21"/>
       <c r="N5" s="21"/>
       <c r="O5" s="21"/>
+      <c r="R5" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="S5" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="T5" s="43" t="s">
+        <v>32</v>
+      </c>
       <c r="U5" s="21"/>
       <c r="V5" s="21"/>
+      <c r="W5" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="X5" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y5" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z5" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA5" s="43" t="s">
+        <v>32</v>
+      </c>
       <c r="AB5" s="21"/>
       <c r="AC5" s="21"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="23"/>
+      <c r="AD5" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="37"/>
       <c r="C6" s="37"/>
       <c r="D6" s="37"/>
       <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
       <c r="N6" s="21"/>
@@ -1111,22 +1217,17 @@
       <c r="AB6" s="21"/>
       <c r="AC6" s="21"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
       <c r="N7" s="21"/>
       <c r="O7" s="21"/>
       <c r="U7" s="21"/>
@@ -1134,20 +1235,17 @@
       <c r="AB7" s="21"/>
       <c r="AC7" s="21"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="37"/>
       <c r="N8" s="21"/>
       <c r="O8" s="21"/>
       <c r="U8" s="21"/>
@@ -1155,20 +1253,22 @@
       <c r="AB8" s="21"/>
       <c r="AC8" s="21"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
       <c r="N9" s="21"/>
       <c r="O9" s="21"/>
       <c r="U9" s="21"/>
@@ -1176,9 +1276,9 @@
       <c r="AB9" s="21"/>
       <c r="AC9" s="21"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="45" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
@@ -1187,9 +1287,9 @@
       <c r="H10" s="21"/>
       <c r="I10" s="23"/>
       <c r="J10" s="23"/>
-      <c r="K10" s="37"/>
+      <c r="K10" s="23"/>
       <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
+      <c r="M10" s="37"/>
       <c r="N10" s="21"/>
       <c r="O10" s="21"/>
       <c r="U10" s="21"/>
@@ -1197,9 +1297,9 @@
       <c r="AB10" s="21"/>
       <c r="AC10" s="21"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>27</v>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" s="45" t="s">
+        <v>25</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
@@ -1209,8 +1309,8 @@
       <c r="I11" s="23"/>
       <c r="J11" s="23"/>
       <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
       <c r="N11" s="21"/>
       <c r="O11" s="21"/>
       <c r="U11" s="21"/>
@@ -1218,9 +1318,9 @@
       <c r="AB11" s="21"/>
       <c r="AC11" s="21"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -1234,16 +1334,15 @@
       <c r="M12" s="23"/>
       <c r="N12" s="21"/>
       <c r="O12" s="21"/>
-      <c r="R12" s="39"/>
-      <c r="S12" s="39"/>
       <c r="U12" s="21"/>
       <c r="V12" s="21"/>
       <c r="AB12" s="21"/>
       <c r="AC12" s="21"/>
-      <c r="AD12" s="40"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
       <c r="F13" s="23"/>
@@ -1261,83 +1360,70 @@
       <c r="AB13" s="21"/>
       <c r="AC13" s="21"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
       <c r="N14" s="21"/>
       <c r="O14" s="21"/>
+      <c r="R14" s="39"/>
+      <c r="S14" s="39"/>
       <c r="U14" s="21"/>
       <c r="V14" s="21"/>
       <c r="AB14" s="21"/>
       <c r="AC14" s="21"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="58" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="33"/>
-      <c r="O15" s="33"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="32"/>
-      <c r="R15" s="32"/>
-      <c r="S15" s="32"/>
-      <c r="T15" s="32"/>
+      <c r="AD14" s="39"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
       <c r="U15" s="21"/>
       <c r="V15" s="21"/>
       <c r="AB15" s="21"/>
       <c r="AC15" s="21"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="31"/>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="32"/>
       <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
+      <c r="D16" s="37"/>
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="32"/>
-      <c r="S16" s="32"/>
-      <c r="T16" s="32"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
       <c r="U16" s="21"/>
       <c r="V16" s="21"/>
       <c r="AB16" s="21"/>
       <c r="AC16" s="21"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A17" s="45" t="s">
-        <v>6</v>
+      <c r="A17" s="58" t="s">
+        <v>4</v>
       </c>
       <c r="B17" s="31"/>
       <c r="C17" s="32"/>
@@ -1364,14 +1450,14 @@
       <c r="AC17" s="21"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
-        <v>33</v>
+      <c r="A18" s="45" t="s">
+        <v>5</v>
       </c>
       <c r="B18" s="31"/>
       <c r="C18" s="32"/>
       <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
       <c r="G18" s="33"/>
       <c r="H18" s="33"/>
       <c r="I18" s="32"/>
@@ -1382,6 +1468,10 @@
       <c r="N18" s="33"/>
       <c r="O18" s="33"/>
       <c r="P18" s="32"/>
+      <c r="Q18" s="32"/>
+      <c r="R18" s="32"/>
+      <c r="S18" s="32"/>
+      <c r="T18" s="32"/>
       <c r="U18" s="21"/>
       <c r="V18" s="21"/>
       <c r="AB18" s="21"/>
@@ -1389,13 +1479,13 @@
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B19" s="31"/>
       <c r="C19" s="32"/>
       <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
       <c r="G19" s="33"/>
       <c r="H19" s="33"/>
       <c r="I19" s="32"/>
@@ -1406,8 +1496,8 @@
       <c r="N19" s="33"/>
       <c r="O19" s="33"/>
       <c r="P19" s="32"/>
-      <c r="Q19" s="39"/>
-      <c r="R19" s="39"/>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="32"/>
       <c r="S19" s="32"/>
       <c r="T19" s="32"/>
       <c r="U19" s="21"/>
@@ -1416,8 +1506,8 @@
       <c r="AC19" s="21"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="45" t="s">
-        <v>12</v>
+      <c r="A20" s="44" t="s">
+        <v>33</v>
       </c>
       <c r="B20" s="31"/>
       <c r="C20" s="32"/>
@@ -1426,7 +1516,7 @@
       <c r="F20" s="32"/>
       <c r="G20" s="33"/>
       <c r="H20" s="33"/>
-      <c r="I20" s="37"/>
+      <c r="I20" s="32"/>
       <c r="J20" s="32"/>
       <c r="K20" s="32"/>
       <c r="L20" s="32"/>
@@ -1434,10 +1524,6 @@
       <c r="N20" s="33"/>
       <c r="O20" s="33"/>
       <c r="P20" s="32"/>
-      <c r="Q20" s="32"/>
-      <c r="R20" s="32"/>
-      <c r="S20" s="32"/>
-      <c r="T20" s="32"/>
       <c r="U20" s="21"/>
       <c r="V20" s="21"/>
       <c r="AB20" s="21"/>
@@ -1445,7 +1531,7 @@
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B21" s="31"/>
       <c r="C21" s="32"/>
@@ -1454,7 +1540,7 @@
       <c r="F21" s="32"/>
       <c r="G21" s="33"/>
       <c r="H21" s="33"/>
-      <c r="I21" s="37"/>
+      <c r="I21" s="32"/>
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
       <c r="L21" s="32"/>
@@ -1462,8 +1548,8 @@
       <c r="N21" s="33"/>
       <c r="O21" s="33"/>
       <c r="P21" s="32"/>
-      <c r="Q21" s="32"/>
-      <c r="R21" s="32"/>
+      <c r="Q21" s="39"/>
+      <c r="R21" s="39"/>
       <c r="S21" s="32"/>
       <c r="T21" s="32"/>
       <c r="U21" s="21"/>
@@ -1473,7 +1559,7 @@
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="45" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B22" s="31"/>
       <c r="C22" s="32"/>
@@ -1501,7 +1587,7 @@
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="45" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B23" s="31"/>
       <c r="C23" s="32"/>
@@ -1529,7 +1615,7 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="45" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B24" s="31"/>
       <c r="C24" s="32"/>
@@ -1538,11 +1624,11 @@
       <c r="F24" s="32"/>
       <c r="G24" s="33"/>
       <c r="H24" s="33"/>
-      <c r="I24" s="32"/>
+      <c r="I24" s="37"/>
       <c r="J24" s="32"/>
       <c r="K24" s="32"/>
       <c r="L24" s="32"/>
-      <c r="M24" s="37"/>
+      <c r="M24" s="32"/>
       <c r="N24" s="33"/>
       <c r="O24" s="33"/>
       <c r="P24" s="32"/>
@@ -1557,7 +1643,7 @@
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="45" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B25" s="31"/>
       <c r="C25" s="32"/>
@@ -1566,14 +1652,14 @@
       <c r="F25" s="32"/>
       <c r="G25" s="33"/>
       <c r="H25" s="33"/>
-      <c r="I25" s="32"/>
+      <c r="I25" s="37"/>
       <c r="J25" s="32"/>
       <c r="K25" s="32"/>
       <c r="L25" s="32"/>
       <c r="M25" s="32"/>
       <c r="N25" s="33"/>
       <c r="O25" s="33"/>
-      <c r="P25" s="37"/>
+      <c r="P25" s="32"/>
       <c r="Q25" s="32"/>
       <c r="R25" s="32"/>
       <c r="S25" s="32"/>
@@ -1584,108 +1670,136 @@
       <c r="AC25" s="21"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A26" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="34"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="35"/>
-      <c r="O26" s="35"/>
-      <c r="P26" s="37"/>
-      <c r="Q26" s="7"/>
-      <c r="R26" s="7"/>
-      <c r="S26" s="7"/>
-      <c r="T26" s="7"/>
+      <c r="A26" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="31"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="33"/>
+      <c r="O26" s="33"/>
+      <c r="P26" s="32"/>
+      <c r="Q26" s="32"/>
+      <c r="R26" s="32"/>
+      <c r="S26" s="32"/>
+      <c r="T26" s="32"/>
       <c r="U26" s="21"/>
       <c r="V26" s="21"/>
       <c r="AB26" s="21"/>
       <c r="AC26" s="21"/>
     </row>
-    <row r="27" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="26"/>
-      <c r="P27" s="25"/>
-      <c r="Q27" s="25"/>
-      <c r="R27" s="25"/>
-      <c r="S27" s="25"/>
-      <c r="T27" s="25"/>
-      <c r="U27" s="26"/>
-      <c r="V27" s="26"/>
-      <c r="W27" s="25"/>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A27" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="31"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="33"/>
+      <c r="O27" s="33"/>
+      <c r="P27" s="37"/>
+      <c r="Q27" s="32"/>
+      <c r="R27" s="32"/>
+      <c r="S27" s="32"/>
+      <c r="T27" s="32"/>
+      <c r="U27" s="21"/>
+      <c r="V27" s="21"/>
       <c r="AB27" s="21"/>
       <c r="AC27" s="21"/>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="N28" s="21"/>
-      <c r="O28" s="21"/>
-      <c r="Q28" s="23"/>
+      <c r="A28" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="34"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="35"/>
+      <c r="O28" s="35"/>
+      <c r="P28" s="37"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
       <c r="U28" s="21"/>
       <c r="V28" s="21"/>
-      <c r="W28" s="37"/>
       <c r="AB28" s="21"/>
       <c r="AC28" s="21"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="N29" s="21"/>
-      <c r="O29" s="21"/>
-      <c r="U29" s="21"/>
-      <c r="V29" s="21"/>
-      <c r="W29" s="23"/>
+    <row r="29" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="25"/>
+      <c r="N29" s="26"/>
+      <c r="O29" s="26"/>
+      <c r="P29" s="25"/>
+      <c r="Q29" s="25"/>
+      <c r="R29" s="25"/>
+      <c r="S29" s="25"/>
+      <c r="T29" s="25"/>
+      <c r="U29" s="26"/>
+      <c r="V29" s="26"/>
+      <c r="W29" s="25"/>
       <c r="AB29" s="21"/>
       <c r="AC29" s="21"/>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
-        <v>22</v>
+      <c r="A30" s="28" t="s">
+        <v>56</v>
       </c>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
       <c r="N30" s="21"/>
       <c r="O30" s="21"/>
+      <c r="Q30" s="23"/>
       <c r="U30" s="21"/>
       <c r="V30" s="21"/>
-      <c r="W30" s="23"/>
+      <c r="W30" s="37"/>
       <c r="AB30" s="21"/>
       <c r="AC30" s="21"/>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G31" s="21"/>
       <c r="H31" s="21"/>
@@ -1693,12 +1807,13 @@
       <c r="O31" s="21"/>
       <c r="U31" s="21"/>
       <c r="V31" s="21"/>
+      <c r="W31" s="23"/>
       <c r="AB31" s="21"/>
       <c r="AC31" s="21"/>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="G32" s="21"/>
       <c r="H32" s="21"/>
@@ -1706,12 +1821,13 @@
       <c r="O32" s="21"/>
       <c r="U32" s="21"/>
       <c r="V32" s="21"/>
+      <c r="W32" s="23"/>
       <c r="AB32" s="21"/>
       <c r="AC32" s="21"/>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33" s="29" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G33" s="21"/>
       <c r="H33" s="21"/>
@@ -1721,10 +1837,11 @@
       <c r="V33" s="21"/>
       <c r="AB33" s="21"/>
       <c r="AC33" s="21"/>
-      <c r="AD33" s="41"/>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
+      <c r="A34" s="29" t="s">
+        <v>31</v>
+      </c>
       <c r="G34" s="21"/>
       <c r="H34" s="21"/>
       <c r="N34" s="21"/>
@@ -1735,8 +1852,8 @@
       <c r="AC34" s="21"/>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
-        <v>30</v>
+      <c r="A35" s="29" t="s">
+        <v>29</v>
       </c>
       <c r="G35" s="21"/>
       <c r="H35" s="21"/>
@@ -1746,8 +1863,10 @@
       <c r="V35" s="21"/>
       <c r="AB35" s="21"/>
       <c r="AC35" s="21"/>
+      <c r="AD35" s="37"/>
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A36" s="22"/>
       <c r="G36" s="21"/>
       <c r="H36" s="21"/>
       <c r="N36" s="21"/>
@@ -1756,9 +1875,11 @@
       <c r="V36" s="21"/>
       <c r="AB36" s="21"/>
       <c r="AC36" s="21"/>
-      <c r="AD36" s="41"/>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="G37" s="21"/>
       <c r="H37" s="21"/>
       <c r="N37" s="21"/>
@@ -1767,7 +1888,6 @@
       <c r="V37" s="21"/>
       <c r="AB37" s="21"/>
       <c r="AC37" s="21"/>
-      <c r="AD37" s="41"/>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="G38" s="21"/>
@@ -1778,6 +1898,28 @@
       <c r="V38" s="21"/>
       <c r="AB38" s="21"/>
       <c r="AC38" s="21"/>
+      <c r="AD38" s="23"/>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="21"/>
+      <c r="U39" s="21"/>
+      <c r="V39" s="21"/>
+      <c r="AB39" s="21"/>
+      <c r="AC39" s="21"/>
+      <c r="AD39" s="23"/>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="21"/>
+      <c r="U40" s="21"/>
+      <c r="V40" s="21"/>
+      <c r="AB40" s="21"/>
+      <c r="AC40" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1787,10 +1929,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AF30"/>
+  <dimension ref="A1:AH30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:I11"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1799,7 +1942,31 @@
     <col min="2" max="32" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:32" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1">
+        <v>8</v>
+      </c>
+      <c r="C1">
+        <v>8</v>
+      </c>
+      <c r="D1">
+        <v>8</v>
+      </c>
+      <c r="E1">
+        <v>8</v>
+      </c>
+      <c r="G1">
+        <v>8</v>
+      </c>
+      <c r="AH1">
+        <f>SUM(B1:AF1)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="10">
         <v>44621</v>
@@ -1895,7 +2062,7 @@
         <v>44651</v>
       </c>
     </row>
-    <row r="3" spans="1:32" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -1909,8 +2076,12 @@
       <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="H3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1926,8 +2097,12 @@
       <c r="L3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
+      <c r="M3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="O3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1975,91 +2150,91 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
         <v>58</v>
       </c>
       <c r="D5" s="39"/>
       <c r="E5" s="39"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="45" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="45" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="45" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="45" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="45" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="45" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="45" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="46" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="30" t="s">
         <v>19</v>
       </c>
@@ -2075,7 +2250,7 @@
       <c r="K20" s="25"/>
       <c r="L20" s="27"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="58" t="s">
         <v>56</v>
       </c>
@@ -2084,56 +2259,57 @@
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L22" s="41"/>
+      <c r="M22" s="41"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="41"/>
-      <c r="I23" s="41"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L23" s="41"/>
+      <c r="M23" s="41"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="I24" s="41"/>
-      <c r="J24" s="41"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
         <v>29</v>
       </c>
       <c r="D26" s="37"/>
       <c r="E26" s="37"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J29" s="41"/>
-      <c r="K29" s="41"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J30" s="41"/>
-      <c r="K30" s="41"/>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="G27" s="37"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N29" s="41"/>
+      <c r="O29" s="41"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N30" s="41"/>
+      <c r="O30" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2542,4 +2718,263 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="61" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="60" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="60" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="64">
+        <v>44631</v>
+      </c>
+      <c r="B4" s="65">
+        <v>0.375</v>
+      </c>
+      <c r="C4" s="65">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D4" s="65">
+        <f>SUM(C4-B4)</f>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="E4" s="66" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="64"/>
+      <c r="B5" s="67">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C5" s="67">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D5" s="65">
+        <f t="shared" ref="D5:D18" si="0">SUM(C5-B5)</f>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E5" s="66" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="66"/>
+      <c r="B6" s="67">
+        <f>C5</f>
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="C6" s="67">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D6" s="65">
+        <f t="shared" si="0"/>
+        <v>3.4722222222222654E-3</v>
+      </c>
+      <c r="E6" s="66" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="66"/>
+      <c r="B7" s="67">
+        <f t="shared" ref="B7:B18" si="1">C6</f>
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="C7" s="67">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D7" s="65">
+        <f t="shared" si="0"/>
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="66"/>
+      <c r="B8" s="67">
+        <f t="shared" si="1"/>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C8" s="67">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="65">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="E8" s="66" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="66"/>
+      <c r="B9" s="67">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="C9" s="67">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="D9" s="65">
+        <f t="shared" si="0"/>
+        <v>7.291666666666663E-2</v>
+      </c>
+      <c r="E9" s="66" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="66"/>
+      <c r="B10" s="67">
+        <f t="shared" si="1"/>
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="C10" s="67">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="D10" s="65">
+        <f t="shared" si="0"/>
+        <v>1.736111111111116E-2</v>
+      </c>
+      <c r="E10" s="66" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="66"/>
+      <c r="B11" s="67">
+        <f t="shared" si="1"/>
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="C11" s="67">
+        <v>0.625000000000001</v>
+      </c>
+      <c r="D11" s="65">
+        <f t="shared" si="0"/>
+        <v>3.4722222222223209E-2</v>
+      </c>
+      <c r="E11" s="66" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="66"/>
+      <c r="B12" s="67">
+        <f t="shared" si="1"/>
+        <v>0.625000000000001</v>
+      </c>
+      <c r="C12" s="67">
+        <v>0.66666666666666796</v>
+      </c>
+      <c r="D12" s="65">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666963E-2</v>
+      </c>
+      <c r="E12" s="66" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="66"/>
+      <c r="B13" s="67">
+        <f t="shared" si="1"/>
+        <v>0.66666666666666796</v>
+      </c>
+      <c r="C13" s="67">
+        <v>0.70833333333333504</v>
+      </c>
+      <c r="D13" s="65">
+        <f t="shared" si="0"/>
+        <v>4.1666666666667074E-2</v>
+      </c>
+      <c r="E13" s="66"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="66"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="66"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="66"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="66"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="66"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="66"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="66"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="66"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="66"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="66"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="63">
+        <f>SUM(D4:D19)</f>
+        <v>0.33333333333333504</v>
+      </c>
+      <c r="E20" s="62"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
v0.024 Fixed Manager + Player Update, still error in Player Update call to API.
</commit_message>
<xml_diff>
--- a/FBM-planning.xlsx
+++ b/FBM-planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="21075" windowHeight="12345" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18960" windowHeight="12045" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Feb" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="94">
   <si>
     <t>M</t>
   </si>
@@ -233,9 +233,6 @@
     <t>Jobbsök/Uppföljning - Agio</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Excelfix tidrapport</t>
   </si>
   <si>
@@ -249,6 +246,60 @@
   </si>
   <si>
     <t>Paus</t>
+  </si>
+  <si>
+    <t>Setting up menu structure</t>
+  </si>
+  <si>
+    <t>Show menu 1 - Sell/Print players skeleton</t>
+  </si>
+  <si>
+    <t>Show menu 2 - Print score skeleton</t>
+  </si>
+  <si>
+    <t>Show menu 5 - Display League table skeleton</t>
+  </si>
+  <si>
+    <t>Setup ManagedTeam</t>
+  </si>
+  <si>
+    <t>FBM setup team with players</t>
+  </si>
+  <si>
+    <t>Ute Vindskivor</t>
+  </si>
+  <si>
+    <t>Misc</t>
+  </si>
+  <si>
+    <t>Misc Total</t>
+  </si>
+  <si>
+    <t>Jobbsök aktiviteter</t>
+  </si>
+  <si>
+    <t>Total dev</t>
+  </si>
+  <si>
+    <t>Excel fix</t>
+  </si>
+  <si>
+    <t>Funct to copy Team Id to db table Players</t>
+  </si>
+  <si>
+    <t>Error in GetPlayerByTeamName</t>
+  </si>
+  <si>
+    <t>handla, lunch</t>
+  </si>
+  <si>
+    <t>Error in Player API</t>
+  </si>
+  <si>
+    <t>Fix Manager + Player Update</t>
+  </si>
+  <si>
+    <t>Rekreation</t>
   </si>
 </sst>
 </file>
@@ -257,7 +308,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-41D]dd/mmm;@"/>
-    <numFmt numFmtId="168" formatCode="hh:mm;@"/>
+    <numFmt numFmtId="165" formatCode="hh:mm;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -291,7 +342,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,6 +442,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,7 +613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -612,11 +693,38 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="17" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="17" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="18" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="18" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="19" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="19" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="20" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="20" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="20" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="21" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="21" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="21" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1929,16 +2037,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH30"/>
+  <dimension ref="A1:AH31"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="32" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2154,8 +2262,8 @@
       <c r="A4" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
@@ -2191,8 +2299,8 @@
       <c r="A11" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40"/>
+      <c r="N11" s="40"/>
+      <c r="O11" s="40"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
@@ -2219,22 +2327,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="45" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="46" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="30" t="s">
         <v>19</v>
       </c>
@@ -2248,9 +2356,23 @@
       <c r="I20" s="25"/>
       <c r="J20" s="25"/>
       <c r="K20" s="25"/>
-      <c r="L20" s="27"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="25"/>
+      <c r="P20" s="25"/>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="25"/>
+      <c r="S20" s="25"/>
+      <c r="T20" s="25"/>
+      <c r="U20" s="25"/>
+      <c r="V20" s="25"/>
+      <c r="W20" s="25"/>
+      <c r="X20" s="25"/>
+      <c r="Y20" s="25"/>
+      <c r="Z20" s="27"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="58" t="s">
         <v>56</v>
       </c>
@@ -2259,57 +2381,74 @@
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="L22" s="41"/>
-      <c r="M22" s="41"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N22" s="41"/>
+      <c r="O22" s="41"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="L23" s="41"/>
-      <c r="M23" s="41"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N23" s="41"/>
+      <c r="O23" s="41"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="M24" s="41"/>
-      <c r="N24" s="41"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O24" s="41"/>
+      <c r="P24" s="41"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O25" s="41"/>
+      <c r="P25" s="41"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
         <v>29</v>
       </c>
       <c r="D26" s="37"/>
       <c r="E26" s="37"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
         <v>59</v>
       </c>
       <c r="G27" s="37"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N29" s="41"/>
+      <c r="N27" s="37"/>
+      <c r="O27" s="41"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="N28" s="37"/>
+      <c r="O28" s="41"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="N29" s="23"/>
       <c r="O29" s="41"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N30" s="41"/>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="O30" s="41"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="N31" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2722,17 +2861,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:D18"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2741,238 +2880,1154 @@
       </c>
     </row>
     <row r="3" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="91" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="60" t="s">
+      <c r="E3" s="91" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="64">
+      <c r="A4" s="81">
         <v>44631</v>
       </c>
-      <c r="B4" s="65">
+      <c r="B4" s="82">
         <v>0.375</v>
       </c>
-      <c r="C4" s="65">
+      <c r="C4" s="82">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D4" s="65">
+      <c r="D4" s="82">
         <f>SUM(C4-B4)</f>
         <v>4.1666666666666685E-2</v>
       </c>
-      <c r="E4" s="66" t="s">
+      <c r="E4" s="83" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="64"/>
-      <c r="B5" s="67">
+      <c r="A5" s="81"/>
+      <c r="B5" s="84">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C5" s="67">
+      <c r="C5" s="84">
         <v>0.42708333333333331</v>
       </c>
-      <c r="D5" s="65">
-        <f t="shared" ref="D5:D18" si="0">SUM(C5-B5)</f>
+      <c r="D5" s="82">
+        <f t="shared" ref="D5:D11" si="0">SUM(C5-B5)</f>
         <v>1.041666666666663E-2</v>
       </c>
-      <c r="E5" s="66" t="s">
+      <c r="E5" s="83" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="66"/>
-      <c r="B6" s="67">
+      <c r="A6" s="83"/>
+      <c r="B6" s="84">
         <f>C5</f>
         <v>0.42708333333333331</v>
       </c>
-      <c r="C6" s="67">
+      <c r="C6" s="84">
         <v>0.43055555555555558</v>
       </c>
-      <c r="D6" s="65">
+      <c r="D6" s="82">
         <f t="shared" si="0"/>
         <v>3.4722222222222654E-3</v>
       </c>
-      <c r="E6" s="66" t="s">
-        <v>72</v>
+      <c r="E6" s="83" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="66"/>
-      <c r="B7" s="67">
-        <f t="shared" ref="B7:B18" si="1">C6</f>
+      <c r="A7" s="83"/>
+      <c r="B7" s="84">
+        <f t="shared" ref="B7:B11" si="1">C6</f>
         <v>0.43055555555555558</v>
       </c>
-      <c r="C7" s="67">
+      <c r="C7" s="84">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D7" s="65">
+      <c r="D7" s="82">
         <f t="shared" si="0"/>
         <v>2.7777777777777735E-2</v>
       </c>
-      <c r="E7" s="38" t="s">
-        <v>73</v>
+      <c r="E7" s="85" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="66"/>
-      <c r="B8" s="67">
+      <c r="A8" s="83"/>
+      <c r="B8" s="84">
         <f t="shared" si="1"/>
         <v>0.45833333333333331</v>
       </c>
-      <c r="C8" s="67">
+      <c r="C8" s="84">
         <v>0.5</v>
       </c>
-      <c r="D8" s="65">
+      <c r="D8" s="82">
         <f t="shared" si="0"/>
         <v>4.1666666666666685E-2</v>
       </c>
-      <c r="E8" s="66" t="s">
+      <c r="E8" s="83" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="66"/>
-      <c r="B9" s="67">
+      <c r="A9" s="67"/>
+      <c r="B9" s="68">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="C9" s="67">
+      <c r="C9" s="68">
         <v>0.57291666666666663</v>
       </c>
-      <c r="D9" s="65">
+      <c r="D9" s="69">
         <f t="shared" si="0"/>
         <v>7.291666666666663E-2</v>
       </c>
-      <c r="E9" s="66" t="s">
-        <v>74</v>
+      <c r="E9" s="67" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="66"/>
-      <c r="B10" s="67">
+      <c r="A10" s="83"/>
+      <c r="B10" s="84">
         <f t="shared" si="1"/>
         <v>0.57291666666666663</v>
       </c>
-      <c r="C10" s="67">
+      <c r="C10" s="84">
         <v>0.59027777777777779</v>
       </c>
-      <c r="D10" s="65">
+      <c r="D10" s="82">
         <f t="shared" si="0"/>
         <v>1.736111111111116E-2</v>
       </c>
-      <c r="E10" s="66" t="s">
-        <v>75</v>
+      <c r="E10" s="83" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="66"/>
-      <c r="B11" s="67">
+      <c r="A11" s="83"/>
+      <c r="B11" s="84">
         <f t="shared" si="1"/>
         <v>0.59027777777777779</v>
       </c>
-      <c r="C11" s="67">
+      <c r="C11" s="84">
         <v>0.625000000000001</v>
       </c>
-      <c r="D11" s="65">
+      <c r="D11" s="82">
         <f t="shared" si="0"/>
         <v>3.4722222222223209E-2</v>
       </c>
-      <c r="E11" s="66" t="s">
+      <c r="E11" s="83" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="66"/>
-      <c r="B12" s="67">
-        <f t="shared" si="1"/>
-        <v>0.625000000000001</v>
-      </c>
-      <c r="C12" s="67">
-        <v>0.66666666666666796</v>
-      </c>
-      <c r="D12" s="65">
-        <f t="shared" si="0"/>
-        <v>4.1666666666666963E-2</v>
-      </c>
-      <c r="E12" s="66" t="s">
+      <c r="A12" s="86"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="86"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="70" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="71"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="72">
+        <f>D9</f>
+        <v>7.291666666666663E-2</v>
+      </c>
+      <c r="E13" s="70"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="65"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="65"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="79" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="80"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="78">
+        <f>SUM(D4:D11)-D9</f>
+        <v>0.17708333333333437</v>
+      </c>
+      <c r="E15" s="79"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="65"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="65"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="62" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="62"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="63">
+        <f>SUM(D4:D11)-(D13+D15)</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="62"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="89"/>
+      <c r="B18" s="89"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="90"/>
+      <c r="E18" s="89"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="91" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="91" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="73">
+        <v>44633</v>
+      </c>
+      <c r="B21" s="74">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C21" s="74">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="74">
+        <f>SUM(C21-B21)</f>
+        <v>8.3333333333333315E-2</v>
+      </c>
+      <c r="E21" s="75" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="66"/>
-      <c r="B13" s="67">
-        <f t="shared" si="1"/>
-        <v>0.66666666666666796</v>
-      </c>
-      <c r="C13" s="67">
-        <v>0.70833333333333504</v>
-      </c>
-      <c r="D13" s="65">
-        <f t="shared" si="0"/>
-        <v>4.1666666666667074E-2</v>
-      </c>
-      <c r="E13" s="66"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="66"/>
-      <c r="B14" s="67"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="66"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="66"/>
-      <c r="B15" s="67"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="66"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="66"/>
-      <c r="B16" s="67"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="66"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="66"/>
-      <c r="B17" s="67"/>
-      <c r="C17" s="67"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="66"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="66"/>
-      <c r="B18" s="67"/>
-      <c r="C18" s="67"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="66"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="62"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="63">
-        <f>SUM(D4:D19)</f>
-        <v>0.33333333333333504</v>
-      </c>
-      <c r="E20" s="62"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="73"/>
+      <c r="B22" s="76">
+        <f>C21</f>
+        <v>0.5</v>
+      </c>
+      <c r="C22" s="76">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D22" s="74">
+        <f t="shared" ref="D22:D25" si="2">SUM(C22-B22)</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E22" s="75" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="67" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="68">
+        <f>C22</f>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C23" s="68">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D23" s="69">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="E23" s="67" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="75"/>
+      <c r="B24" s="76">
+        <f t="shared" ref="B24:B25" si="3">C23</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C24" s="76">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D24" s="74">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="E24" s="77" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="67" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="68">
+        <f t="shared" si="3"/>
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C25" s="68">
+        <v>0.875</v>
+      </c>
+      <c r="D25" s="69">
+        <f t="shared" si="2"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E25" s="67" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="65"/>
+      <c r="B26" s="66"/>
+      <c r="C26" s="66"/>
+      <c r="E26" s="65"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="70" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="71"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="72">
+        <f>D23+D25</f>
+        <v>0.20833333333333337</v>
+      </c>
+      <c r="E27" s="70"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="65"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="65"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="93" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="93"/>
+      <c r="C29" s="93"/>
+      <c r="D29" s="94">
+        <f>SUM(D21:D26)-D27</f>
+        <v>0.24999999999999994</v>
+      </c>
+      <c r="E29" s="93"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="91" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="91" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="73">
+        <v>44634</v>
+      </c>
+      <c r="B33" s="74">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C33" s="74">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D33" s="74">
+        <f>SUM(C33-B33)</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E33" s="75" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="73"/>
+      <c r="B34" s="76">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C34" s="76">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D34" s="74">
+        <f t="shared" ref="D34:D40" si="4">SUM(C34-B34)</f>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E34" s="75" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="67"/>
+      <c r="B35" s="68">
+        <f>C34</f>
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="C35" s="68">
+        <v>0.4375</v>
+      </c>
+      <c r="D35" s="69">
+        <f t="shared" si="4"/>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="E35" s="92" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="75"/>
+      <c r="B36" s="76">
+        <f t="shared" ref="B36:B40" si="5">C35</f>
+        <v>0.4375</v>
+      </c>
+      <c r="C36" s="76">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D36" s="74">
+        <f t="shared" si="4"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="E36" s="75" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="67"/>
+      <c r="B37" s="68">
+        <f t="shared" si="5"/>
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C37" s="68">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D37" s="69">
+        <f t="shared" si="4"/>
+        <v>0.12499999999999994</v>
+      </c>
+      <c r="E37" s="67" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="67"/>
+      <c r="B38" s="68">
+        <f t="shared" si="5"/>
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C38" s="68">
+        <v>0.71875</v>
+      </c>
+      <c r="D38" s="69">
+        <f t="shared" si="4"/>
+        <v>0.11458333333333337</v>
+      </c>
+      <c r="E38" s="67" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="75"/>
+      <c r="B39" s="76">
+        <f t="shared" si="5"/>
+        <v>0.71875</v>
+      </c>
+      <c r="C39" s="76">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D39" s="74">
+        <f t="shared" si="4"/>
+        <v>7.291666666666663E-2</v>
+      </c>
+      <c r="E39" s="75" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="75"/>
+      <c r="B40" s="76">
+        <f t="shared" si="5"/>
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C40" s="76">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="D40" s="74">
+        <f t="shared" si="4"/>
+        <v>0.10416666666666674</v>
+      </c>
+      <c r="E40" s="75" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="86"/>
+      <c r="B41" s="87"/>
+      <c r="C41" s="87"/>
+      <c r="D41" s="88"/>
+      <c r="E41" s="86"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="70" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="71"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="72">
+        <f>D35+D37+D38</f>
+        <v>0.25</v>
+      </c>
+      <c r="E42" s="70"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="65"/>
+      <c r="B43" s="66"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="64"/>
+      <c r="E43" s="65"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="79" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="80"/>
+      <c r="C44" s="80"/>
+      <c r="D44" s="78"/>
+      <c r="E44" s="79"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="65"/>
+      <c r="B45" s="66"/>
+      <c r="C45" s="66"/>
+      <c r="D45" s="64"/>
+      <c r="E45" s="65"/>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="93" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" s="93"/>
+      <c r="C46" s="93"/>
+      <c r="D46" s="94">
+        <f>SUM(D33:D40)-(D42+D44)</f>
+        <v>0.3125</v>
+      </c>
+      <c r="E46" s="93"/>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="B49" s="91" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D49" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="E49" s="91" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="73">
+        <v>44635</v>
+      </c>
+      <c r="B50" s="74">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C50" s="74">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D50" s="74">
+        <f>SUM(C50-B50)</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E50" s="75"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="73"/>
+      <c r="B51" s="76">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C51" s="74">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D51" s="74">
+        <f t="shared" ref="D51:D57" si="6">SUM(C51-B51)</f>
+        <v>0</v>
+      </c>
+      <c r="E51" s="75"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="67"/>
+      <c r="B52" s="68">
+        <v>0.5</v>
+      </c>
+      <c r="C52" s="69">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D52" s="69">
+        <f t="shared" si="6"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E52" s="92" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="75"/>
+      <c r="B53" s="76">
+        <f t="shared" ref="B53:B57" si="7">C52</f>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C53" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D53" s="74">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E53" s="75"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="75"/>
+      <c r="B54" s="76">
+        <f t="shared" si="7"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C54" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D54" s="74">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E54" s="75"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="75"/>
+      <c r="B55" s="76">
+        <f t="shared" si="7"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C55" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D55" s="74">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E55" s="75"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="75"/>
+      <c r="B56" s="76">
+        <f t="shared" si="7"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C56" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D56" s="74">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E56" s="75"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="75"/>
+      <c r="B57" s="76">
+        <f t="shared" si="7"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C57" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D57" s="74">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E57" s="75"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="86"/>
+      <c r="B58" s="87"/>
+      <c r="C58" s="87"/>
+      <c r="D58" s="88"/>
+      <c r="E58" s="86"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="70" t="s">
+        <v>84</v>
+      </c>
+      <c r="B59" s="71"/>
+      <c r="C59" s="71"/>
+      <c r="D59" s="72">
+        <f>D52+D54+D55</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E59" s="70"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="65"/>
+      <c r="B60" s="66"/>
+      <c r="C60" s="66"/>
+      <c r="D60" s="64"/>
+      <c r="E60" s="65"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="79" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" s="80"/>
+      <c r="C61" s="80"/>
+      <c r="D61" s="78"/>
+      <c r="E61" s="79"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="65"/>
+      <c r="B62" s="66"/>
+      <c r="C62" s="66"/>
+      <c r="D62" s="64"/>
+      <c r="E62" s="65"/>
+    </row>
+    <row r="63" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="93" t="s">
+        <v>86</v>
+      </c>
+      <c r="B63" s="93"/>
+      <c r="C63" s="93"/>
+      <c r="D63" s="94">
+        <f>SUM(D50:D57)-(D59+D61)</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E63" s="93"/>
+    </row>
+    <row r="64" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="B66" s="91" t="s">
+        <v>65</v>
+      </c>
+      <c r="C66" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D66" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="E66" s="91" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="73">
+        <v>44636</v>
+      </c>
+      <c r="B67" s="74">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C67" s="74">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D67" s="74">
+        <f>SUM(C67-B67)</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E67" s="75"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="73"/>
+      <c r="B68" s="76">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C68" s="74">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D68" s="74">
+        <f t="shared" ref="D68:D74" si="8">SUM(C68-B68)</f>
+        <v>0</v>
+      </c>
+      <c r="E68" s="75"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="67"/>
+      <c r="B69" s="68">
+        <v>0.5</v>
+      </c>
+      <c r="C69" s="69">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D69" s="69">
+        <f t="shared" si="8"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E69" s="92" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="75"/>
+      <c r="B70" s="76">
+        <f t="shared" ref="B70:B74" si="9">C69</f>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C70" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D70" s="74">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E70" s="75"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="75"/>
+      <c r="B71" s="76">
+        <f t="shared" si="9"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C71" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D71" s="74">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E71" s="75"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="75"/>
+      <c r="B72" s="76">
+        <f t="shared" si="9"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C72" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D72" s="74">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E72" s="75"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="75"/>
+      <c r="B73" s="76">
+        <f t="shared" si="9"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C73" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D73" s="74">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E73" s="75"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="75"/>
+      <c r="B74" s="76">
+        <f t="shared" si="9"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C74" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D74" s="74">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E74" s="75"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="86"/>
+      <c r="B75" s="87"/>
+      <c r="C75" s="87"/>
+      <c r="D75" s="88"/>
+      <c r="E75" s="86"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="70" t="s">
+        <v>84</v>
+      </c>
+      <c r="B76" s="71"/>
+      <c r="C76" s="71"/>
+      <c r="D76" s="72">
+        <f>D69+D71+D72</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E76" s="70"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="65"/>
+      <c r="B77" s="66"/>
+      <c r="C77" s="66"/>
+      <c r="D77" s="64"/>
+      <c r="E77" s="65"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="79" t="s">
+        <v>85</v>
+      </c>
+      <c r="B78" s="80"/>
+      <c r="C78" s="80"/>
+      <c r="D78" s="78"/>
+      <c r="E78" s="79"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="65"/>
+      <c r="B79" s="66"/>
+      <c r="C79" s="66"/>
+      <c r="D79" s="64"/>
+      <c r="E79" s="65"/>
+    </row>
+    <row r="80" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="93" t="s">
+        <v>86</v>
+      </c>
+      <c r="B80" s="93"/>
+      <c r="C80" s="93"/>
+      <c r="D80" s="94">
+        <f>SUM(D67:D74)-(D76+D78)</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E80" s="93"/>
+    </row>
+    <row r="81" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="B83" s="91" t="s">
+        <v>65</v>
+      </c>
+      <c r="C83" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D83" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="E83" s="91" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="73">
+        <v>44637</v>
+      </c>
+      <c r="B84" s="74">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C84" s="74">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D84" s="74">
+        <f>SUM(C84-B84)</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E84" s="75"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="73"/>
+      <c r="B85" s="76">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C85" s="74">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D85" s="74">
+        <f t="shared" ref="D85:D91" si="10">SUM(C85-B85)</f>
+        <v>0</v>
+      </c>
+      <c r="E85" s="75"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="67"/>
+      <c r="B86" s="68">
+        <v>0.5</v>
+      </c>
+      <c r="C86" s="69">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D86" s="69">
+        <f t="shared" si="10"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E86" s="92" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="75"/>
+      <c r="B87" s="76">
+        <f t="shared" ref="B87:B91" si="11">C86</f>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C87" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D87" s="74">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E87" s="75"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="75"/>
+      <c r="B88" s="76">
+        <f t="shared" si="11"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C88" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D88" s="74">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E88" s="75"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="75"/>
+      <c r="B89" s="76">
+        <f t="shared" si="11"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C89" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D89" s="74">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E89" s="75"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="75"/>
+      <c r="B90" s="76">
+        <f t="shared" si="11"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C90" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D90" s="74">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E90" s="75"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="75"/>
+      <c r="B91" s="76">
+        <f t="shared" si="11"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C91" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D91" s="74">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E91" s="75"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="86"/>
+      <c r="B92" s="87"/>
+      <c r="C92" s="87"/>
+      <c r="D92" s="88"/>
+      <c r="E92" s="86"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="70" t="s">
+        <v>84</v>
+      </c>
+      <c r="B93" s="71"/>
+      <c r="C93" s="71"/>
+      <c r="D93" s="72">
+        <f>D86+D88+D89</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E93" s="70"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="65"/>
+      <c r="B94" s="66"/>
+      <c r="C94" s="66"/>
+      <c r="D94" s="64"/>
+      <c r="E94" s="65"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="79" t="s">
+        <v>85</v>
+      </c>
+      <c r="B95" s="80"/>
+      <c r="C95" s="80"/>
+      <c r="D95" s="78"/>
+      <c r="E95" s="79"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="65"/>
+      <c r="B96" s="66"/>
+      <c r="C96" s="66"/>
+      <c r="D96" s="64"/>
+      <c r="E96" s="65"/>
+    </row>
+    <row r="97" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="93" t="s">
+        <v>86</v>
+      </c>
+      <c r="B97" s="93"/>
+      <c r="C97" s="93"/>
+      <c r="D97" s="94">
+        <f>SUM(D84:D91)-(D93+D95)</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E97" s="93"/>
+    </row>
+    <row r="98" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
v0.028 Fixed init ManagedTeam with rnd players from roster
</commit_message>
<xml_diff>
--- a/FBM-planning.xlsx
+++ b/FBM-planning.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="101">
   <si>
     <t>M</t>
   </si>
@@ -300,6 +300,27 @@
   </si>
   <si>
     <t>Rekreation</t>
+  </si>
+  <si>
+    <t>Curonova möte</t>
+  </si>
+  <si>
+    <t>Update error 500 from frontend</t>
+  </si>
+  <si>
+    <t>Jobbsök</t>
+  </si>
+  <si>
+    <t>Middag</t>
+  </si>
+  <si>
+    <t>fix Manager + Player Update API call</t>
+  </si>
+  <si>
+    <t>fix all new Player Update API call, now working!</t>
+  </si>
+  <si>
+    <t>changed to a completely new function</t>
   </si>
 </sst>
 </file>
@@ -613,7 +634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -725,6 +746,8 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="18" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2861,17 +2884,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E98"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.85546875" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3402,16 +3425,16 @@
       <c r="E41" s="86"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="70" t="s">
+      <c r="A42" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="B42" s="71"/>
-      <c r="C42" s="71"/>
-      <c r="D42" s="72">
+      <c r="B42" s="68"/>
+      <c r="C42" s="68"/>
+      <c r="D42" s="69">
         <f>D35+D37+D38</f>
         <v>0.25</v>
       </c>
-      <c r="E42" s="70"/>
+      <c r="E42" s="67"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="65"/>
@@ -3474,260 +3497,276 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="C50" s="74">
-        <v>0.41666666666666669</v>
+        <v>0.40277777777777773</v>
       </c>
       <c r="D50" s="74">
         <f>SUM(C50-B50)</f>
-        <v>8.333333333333337E-2</v>
-      </c>
-      <c r="E50" s="75"/>
+        <v>6.944444444444442E-2</v>
+      </c>
+      <c r="E50" s="75" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="73"/>
-      <c r="B51" s="76">
+      <c r="A51" s="96"/>
+      <c r="B51" s="69">
+        <f>C50</f>
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="C51" s="69">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C51" s="74">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="D51" s="74">
-        <f t="shared" ref="D51:D57" si="6">SUM(C51-B51)</f>
-        <v>0</v>
-      </c>
-      <c r="E51" s="75"/>
+      <c r="D51" s="69">
+        <f>SUM(C51-B51)</f>
+        <v>1.3888888888888951E-2</v>
+      </c>
+      <c r="E51" s="67" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="67"/>
-      <c r="B52" s="68">
+      <c r="A52" s="95"/>
+      <c r="B52" s="80">
+        <f>C50</f>
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="C52" s="78">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D52" s="78">
+        <f t="shared" ref="D52:D58" si="6">SUM(C52-B52)</f>
+        <v>5.555555555555558E-2</v>
+      </c>
+      <c r="E52" s="79" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="67"/>
+      <c r="B53" s="68">
         <v>0.5</v>
       </c>
-      <c r="C52" s="69">
+      <c r="C53" s="69">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D52" s="69">
+      <c r="D53" s="69">
         <f t="shared" si="6"/>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="E52" s="92" t="s">
+      <c r="E53" s="92" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="75"/>
-      <c r="B53" s="76">
-        <f t="shared" ref="B53:B57" si="7">C52</f>
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C53" s="74">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D53" s="74">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E53" s="75"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="75"/>
       <c r="B54" s="76">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="B54:B57" si="7">C53</f>
         <v>0.54166666666666663</v>
       </c>
       <c r="C54" s="74">
-        <v>0.54166666666666663</v>
+        <v>0.61458333333333337</v>
       </c>
       <c r="D54" s="74">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E54" s="75"/>
+        <v>7.2916666666666741E-2</v>
+      </c>
+      <c r="E54" s="75" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="75"/>
-      <c r="B55" s="76">
+      <c r="A55" s="79"/>
+      <c r="B55" s="80">
         <f t="shared" si="7"/>
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C55" s="74">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D55" s="74">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="C55" s="78">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D55" s="78">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E55" s="75"/>
+        <v>5.2083333333333259E-2</v>
+      </c>
+      <c r="E55" s="79" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="75"/>
-      <c r="B56" s="76">
+      <c r="A56" s="67"/>
+      <c r="B56" s="68">
         <f t="shared" si="7"/>
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C56" s="74">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D56" s="74">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C56" s="69">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="D56" s="69">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E56" s="75"/>
+        <v>7.2916666666666741E-2</v>
+      </c>
+      <c r="E56" s="67" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="75"/>
       <c r="B57" s="76">
         <f t="shared" si="7"/>
-        <v>0.54166666666666663</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="C57" s="74">
-        <v>0.54166666666666663</v>
+        <v>0.875</v>
       </c>
       <c r="D57" s="74">
         <f t="shared" si="6"/>
+        <v>0.13541666666666663</v>
+      </c>
+      <c r="E57" s="75" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="75"/>
+      <c r="B58" s="76"/>
+      <c r="C58" s="74"/>
+      <c r="D58" s="74">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="E57" s="75"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="86"/>
-      <c r="B58" s="87"/>
-      <c r="C58" s="87"/>
-      <c r="D58" s="88"/>
-      <c r="E58" s="86"/>
+      <c r="E58" s="75" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="70" t="s">
+      <c r="A59" s="86"/>
+      <c r="B59" s="87"/>
+      <c r="C59" s="87"/>
+      <c r="D59" s="88"/>
+      <c r="E59" s="86"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="B59" s="71"/>
-      <c r="C59" s="71"/>
-      <c r="D59" s="72">
-        <f>D52+D54+D55</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-      <c r="E59" s="70"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="65"/>
-      <c r="B60" s="66"/>
-      <c r="C60" s="66"/>
-      <c r="D60" s="64"/>
-      <c r="E60" s="65"/>
+      <c r="B60" s="68"/>
+      <c r="C60" s="68"/>
+      <c r="D60" s="69">
+        <f>D51+D53+D56</f>
+        <v>0.12847222222222232</v>
+      </c>
+      <c r="E60" s="67"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="79" t="s">
+      <c r="A61" s="65"/>
+      <c r="B61" s="66"/>
+      <c r="C61" s="66"/>
+      <c r="D61" s="64"/>
+      <c r="E61" s="65"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="B61" s="80"/>
-      <c r="C61" s="80"/>
-      <c r="D61" s="78"/>
-      <c r="E61" s="79"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="65"/>
-      <c r="B62" s="66"/>
-      <c r="C62" s="66"/>
-      <c r="D62" s="64"/>
-      <c r="E62" s="65"/>
-    </row>
-    <row r="63" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="93" t="s">
+      <c r="B62" s="80"/>
+      <c r="C62" s="80"/>
+      <c r="D62" s="78">
+        <f>D52+D55</f>
+        <v>0.10763888888888884</v>
+      </c>
+      <c r="E62" s="79"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="65"/>
+      <c r="B63" s="66"/>
+      <c r="C63" s="66"/>
+      <c r="D63" s="64"/>
+      <c r="E63" s="65"/>
+    </row>
+    <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="93" t="s">
         <v>86</v>
       </c>
-      <c r="B63" s="93"/>
-      <c r="C63" s="93"/>
-      <c r="D63" s="94">
-        <f>SUM(D50:D57)-(D59+D61)</f>
+      <c r="B64" s="93"/>
+      <c r="C64" s="93"/>
+      <c r="D64" s="94">
+        <f>SUM(D50:D58)-(D60+D62)</f>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="E64" s="93"/>
+    </row>
+    <row r="65" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="B67" s="91" t="s">
+        <v>65</v>
+      </c>
+      <c r="C67" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D67" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="E67" s="91" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="73">
+        <v>44636</v>
+      </c>
+      <c r="B68" s="74">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C68" s="74">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D68" s="74">
+        <f>SUM(C68-B68)</f>
+        <v>0</v>
+      </c>
+      <c r="E68" s="75"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="73"/>
+      <c r="B69" s="76">
+        <f>C68</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C69" s="74">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D69" s="74">
+        <f t="shared" ref="D69:D75" si="8">SUM(C69-B69)</f>
+        <v>0</v>
+      </c>
+      <c r="E69" s="75"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="67"/>
+      <c r="B70" s="68">
+        <v>0.5</v>
+      </c>
+      <c r="C70" s="69">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D70" s="69">
+        <f t="shared" si="8"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E63" s="93"/>
-    </row>
-    <row r="64" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="91" t="s">
-        <v>64</v>
-      </c>
-      <c r="B66" s="91" t="s">
-        <v>65</v>
-      </c>
-      <c r="C66" s="91" t="s">
-        <v>66</v>
-      </c>
-      <c r="D66" s="91" t="s">
-        <v>68</v>
-      </c>
-      <c r="E66" s="91" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="73">
-        <v>44636</v>
-      </c>
-      <c r="B67" s="74">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C67" s="74">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="D67" s="74">
-        <f>SUM(C67-B67)</f>
-        <v>8.333333333333337E-2</v>
-      </c>
-      <c r="E67" s="75"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="73"/>
-      <c r="B68" s="76">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="C68" s="74">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="D68" s="74">
-        <f t="shared" ref="D68:D74" si="8">SUM(C68-B68)</f>
-        <v>0</v>
-      </c>
-      <c r="E68" s="75"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="67"/>
-      <c r="B69" s="68">
-        <v>0.5</v>
-      </c>
-      <c r="C69" s="69">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D69" s="69">
-        <f t="shared" si="8"/>
-        <v>4.166666666666663E-2</v>
-      </c>
-      <c r="E69" s="92" t="s">
+      <c r="E70" s="92" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="75"/>
-      <c r="B70" s="76">
-        <f t="shared" ref="B70:B74" si="9">C69</f>
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C70" s="74">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D70" s="74">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="E70" s="75"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="75"/>
       <c r="B71" s="76">
-        <f t="shared" si="9"/>
-        <v>0.54166666666666663</v>
+        <f t="shared" ref="B71:B75" si="9">C70</f>
+        <v>0.58333333333333337</v>
       </c>
       <c r="C71" s="74">
-        <v>0.54166666666666663</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="D71" s="74">
         <f t="shared" si="8"/>
@@ -3739,10 +3778,10 @@
       <c r="A72" s="75"/>
       <c r="B72" s="76">
         <f t="shared" si="9"/>
-        <v>0.54166666666666663</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="C72" s="74">
-        <v>0.54166666666666663</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="D72" s="74">
         <f t="shared" si="8"/>
@@ -3754,10 +3793,10 @@
       <c r="A73" s="75"/>
       <c r="B73" s="76">
         <f t="shared" si="9"/>
-        <v>0.54166666666666663</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="C73" s="74">
-        <v>0.54166666666666663</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="D73" s="74">
         <f t="shared" si="8"/>
@@ -3769,10 +3808,10 @@
       <c r="A74" s="75"/>
       <c r="B74" s="76">
         <f t="shared" si="9"/>
-        <v>0.54166666666666663</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="C74" s="74">
-        <v>0.54166666666666663</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="D74" s="74">
         <f t="shared" si="8"/>
@@ -3781,142 +3820,142 @@
       <c r="E74" s="75"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="86"/>
-      <c r="B75" s="87"/>
-      <c r="C75" s="87"/>
-      <c r="D75" s="88"/>
-      <c r="E75" s="86"/>
+      <c r="A75" s="75"/>
+      <c r="B75" s="76">
+        <f t="shared" si="9"/>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C75" s="74">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D75" s="74">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E75" s="75"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="70" t="s">
+      <c r="A76" s="86"/>
+      <c r="B76" s="87"/>
+      <c r="C76" s="87"/>
+      <c r="D76" s="88"/>
+      <c r="E76" s="86"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="B76" s="71"/>
-      <c r="C76" s="71"/>
-      <c r="D76" s="72">
-        <f>D69+D71+D72</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-      <c r="E76" s="70"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="65"/>
-      <c r="B77" s="66"/>
-      <c r="C77" s="66"/>
-      <c r="D77" s="64"/>
-      <c r="E77" s="65"/>
+      <c r="B77" s="68"/>
+      <c r="C77" s="68"/>
+      <c r="D77" s="69">
+        <f>D70+D72+D73</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E77" s="67"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="79" t="s">
+      <c r="A78" s="65"/>
+      <c r="B78" s="66"/>
+      <c r="C78" s="66"/>
+      <c r="D78" s="64"/>
+      <c r="E78" s="65"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="B78" s="80"/>
-      <c r="C78" s="80"/>
-      <c r="D78" s="78"/>
-      <c r="E78" s="79"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="65"/>
-      <c r="B79" s="66"/>
-      <c r="C79" s="66"/>
-      <c r="D79" s="64"/>
-      <c r="E79" s="65"/>
-    </row>
-    <row r="80" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="93" t="s">
+      <c r="B79" s="80"/>
+      <c r="C79" s="80"/>
+      <c r="D79" s="78"/>
+      <c r="E79" s="79"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="65"/>
+      <c r="B80" s="66"/>
+      <c r="C80" s="66"/>
+      <c r="D80" s="64"/>
+      <c r="E80" s="65"/>
+    </row>
+    <row r="81" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="93" t="s">
         <v>86</v>
       </c>
-      <c r="B80" s="93"/>
-      <c r="C80" s="93"/>
-      <c r="D80" s="94">
-        <f>SUM(D67:D74)-(D76+D78)</f>
-        <v>8.333333333333337E-2</v>
-      </c>
-      <c r="E80" s="93"/>
-    </row>
-    <row r="81" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="91" t="s">
+      <c r="B81" s="93"/>
+      <c r="C81" s="93"/>
+      <c r="D81" s="94">
+        <f>SUM(D68:D75)-(D77+D79)</f>
+        <v>0</v>
+      </c>
+      <c r="E81" s="93"/>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="B83" s="91" t="s">
+      <c r="B84" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="C83" s="91" t="s">
+      <c r="C84" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="D83" s="91" t="s">
+      <c r="D84" s="91" t="s">
         <v>68</v>
       </c>
-      <c r="E83" s="91" t="s">
+      <c r="E84" s="91" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="73">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="73">
         <v>44637</v>
       </c>
-      <c r="B84" s="74">
+      <c r="B85" s="74">
         <v>0.33333333333333331</v>
-      </c>
-      <c r="C84" s="74">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="D84" s="74">
-        <f>SUM(C84-B84)</f>
-        <v>8.333333333333337E-2</v>
-      </c>
-      <c r="E84" s="75"/>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="73"/>
-      <c r="B85" s="76">
-        <v>0.41666666666666669</v>
       </c>
       <c r="C85" s="74">
         <v>0.41666666666666669</v>
       </c>
       <c r="D85" s="74">
-        <f t="shared" ref="D85:D91" si="10">SUM(C85-B85)</f>
+        <f>SUM(C85-B85)</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E85" s="75"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="73"/>
+      <c r="B86" s="76">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C86" s="74">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D86" s="74">
+        <f t="shared" ref="D86:D92" si="10">SUM(C86-B86)</f>
         <v>0</v>
       </c>
-      <c r="E85" s="75"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="67"/>
-      <c r="B86" s="68">
+      <c r="E86" s="75"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="67"/>
+      <c r="B87" s="68">
         <v>0.5</v>
       </c>
-      <c r="C86" s="69">
+      <c r="C87" s="69">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D86" s="69">
+      <c r="D87" s="69">
         <f t="shared" si="10"/>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="E86" s="92" t="s">
+      <c r="E87" s="92" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="75"/>
-      <c r="B87" s="76">
-        <f t="shared" ref="B87:B91" si="11">C86</f>
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C87" s="74">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D87" s="74">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="E87" s="75"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="75"/>
       <c r="B88" s="76">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="B88:B92" si="11">C87</f>
         <v>0.54166666666666663</v>
       </c>
       <c r="C88" s="74">
@@ -3974,60 +4013,75 @@
       <c r="E91" s="75"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="86"/>
-      <c r="B92" s="87"/>
-      <c r="C92" s="87"/>
-      <c r="D92" s="88"/>
-      <c r="E92" s="86"/>
+      <c r="A92" s="75"/>
+      <c r="B92" s="76">
+        <f t="shared" si="11"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C92" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D92" s="74">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E92" s="75"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="70" t="s">
+      <c r="A93" s="86"/>
+      <c r="B93" s="87"/>
+      <c r="C93" s="87"/>
+      <c r="D93" s="88"/>
+      <c r="E93" s="86"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="B93" s="71"/>
-      <c r="C93" s="71"/>
-      <c r="D93" s="72">
-        <f>D86+D88+D89</f>
+      <c r="B94" s="71"/>
+      <c r="C94" s="71"/>
+      <c r="D94" s="72">
+        <f>D87+D89+D90</f>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="E93" s="70"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="65"/>
-      <c r="B94" s="66"/>
-      <c r="C94" s="66"/>
-      <c r="D94" s="64"/>
-      <c r="E94" s="65"/>
+      <c r="E94" s="70"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="79" t="s">
+      <c r="A95" s="65"/>
+      <c r="B95" s="66"/>
+      <c r="C95" s="66"/>
+      <c r="D95" s="64"/>
+      <c r="E95" s="65"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="B95" s="80"/>
-      <c r="C95" s="80"/>
-      <c r="D95" s="78"/>
-      <c r="E95" s="79"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="65"/>
-      <c r="B96" s="66"/>
-      <c r="C96" s="66"/>
-      <c r="D96" s="64"/>
-      <c r="E96" s="65"/>
-    </row>
-    <row r="97" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="93" t="s">
+      <c r="B96" s="80"/>
+      <c r="C96" s="80"/>
+      <c r="D96" s="78"/>
+      <c r="E96" s="79"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="65"/>
+      <c r="B97" s="66"/>
+      <c r="C97" s="66"/>
+      <c r="D97" s="64"/>
+      <c r="E97" s="65"/>
+    </row>
+    <row r="98" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="93" t="s">
         <v>86</v>
       </c>
-      <c r="B97" s="93"/>
-      <c r="C97" s="93"/>
-      <c r="D97" s="94">
-        <f>SUM(D84:D91)-(D93+D95)</f>
+      <c r="B98" s="93"/>
+      <c r="C98" s="93"/>
+      <c r="D98" s="94">
+        <f>SUM(D85:D92)-(D94+D96)</f>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E97" s="93"/>
-    </row>
-    <row r="98" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="E98" s="93"/>
+    </row>
+    <row r="99" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
v0.029 Setup new tests
</commit_message>
<xml_diff>
--- a/FBM-planning.xlsx
+++ b/FBM-planning.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="104">
   <si>
     <t>M</t>
   </si>
@@ -321,6 +321,15 @@
   </si>
   <si>
     <t>changed to a completely new function</t>
+  </si>
+  <si>
+    <t>fix start of game functions(intit manager, team etc.)</t>
+  </si>
+  <si>
+    <t>Huvudvärk</t>
+  </si>
+  <si>
+    <t>Unit testing with xUnit</t>
   </si>
 </sst>
 </file>
@@ -2884,10 +2893,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3726,7 +3735,9 @@
         <f>SUM(C68-B68)</f>
         <v>0</v>
       </c>
-      <c r="E68" s="75"/>
+      <c r="E68" s="75" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="73"/>
@@ -3749,11 +3760,11 @@
         <v>0.5</v>
       </c>
       <c r="C70" s="69">
-        <v>0.58333333333333337</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="D70" s="69">
         <f t="shared" si="8"/>
-        <v>8.333333333333337E-2</v>
+        <v>0.10416666666666663</v>
       </c>
       <c r="E70" s="92" t="s">
         <v>73</v>
@@ -3763,55 +3774,59 @@
       <c r="A71" s="75"/>
       <c r="B71" s="76">
         <f t="shared" ref="B71:B75" si="9">C70</f>
-        <v>0.58333333333333337</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="C71" s="74">
-        <v>0.58333333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D71" s="74">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="E71" s="75"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E71" s="75" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="75"/>
-      <c r="B72" s="76">
+      <c r="A72" s="67"/>
+      <c r="B72" s="68">
         <f t="shared" si="9"/>
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="C72" s="74">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="D72" s="74">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C72" s="69">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="D72" s="69">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="E72" s="75"/>
+        <v>5.555555555555558E-2</v>
+      </c>
+      <c r="E72" s="67"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="75"/>
       <c r="B73" s="76">
         <f t="shared" si="9"/>
-        <v>0.58333333333333337</v>
+        <v>0.72222222222222221</v>
       </c>
       <c r="C73" s="74">
-        <v>0.58333333333333337</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="D73" s="74">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="E73" s="75"/>
+        <v>6.944444444444442E-2</v>
+      </c>
+      <c r="E73" s="75" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="75"/>
       <c r="B74" s="76">
         <f t="shared" si="9"/>
-        <v>0.58333333333333337</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="C74" s="74">
-        <v>0.58333333333333337</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="D74" s="74">
         <f t="shared" si="8"/>
@@ -3823,10 +3838,10 @@
       <c r="A75" s="75"/>
       <c r="B75" s="76">
         <f t="shared" si="9"/>
-        <v>0.58333333333333337</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="C75" s="74">
-        <v>0.58333333333333337</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="D75" s="74">
         <f t="shared" si="8"/>
@@ -3848,8 +3863,8 @@
       <c r="B77" s="68"/>
       <c r="C77" s="68"/>
       <c r="D77" s="69">
-        <f>D70+D72+D73</f>
-        <v>8.333333333333337E-2</v>
+        <f>D70+D72</f>
+        <v>0.15972222222222221</v>
       </c>
       <c r="E77" s="67"/>
     </row>
@@ -3884,7 +3899,7 @@
       <c r="C81" s="93"/>
       <c r="D81" s="94">
         <f>SUM(D68:D75)-(D77+D79)</f>
-        <v>0</v>
+        <v>0.13194444444444442</v>
       </c>
       <c r="E81" s="93"/>
     </row>
@@ -3911,16 +3926,18 @@
         <v>44637</v>
       </c>
       <c r="B85" s="74">
-        <v>0.33333333333333331</v>
+        <v>0.375</v>
       </c>
       <c r="C85" s="74">
         <v>0.41666666666666669</v>
       </c>
       <c r="D85" s="74">
         <f>SUM(C85-B85)</f>
-        <v>8.333333333333337E-2</v>
-      </c>
-      <c r="E85" s="75"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="E85" s="75" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="73"/>
@@ -4035,16 +4052,16 @@
       <c r="E93" s="86"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="70" t="s">
+      <c r="A94" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="B94" s="71"/>
-      <c r="C94" s="71"/>
-      <c r="D94" s="72">
+      <c r="B94" s="68"/>
+      <c r="C94" s="68"/>
+      <c r="D94" s="69">
         <f>D87+D89+D90</f>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="E94" s="70"/>
+      <c r="E94" s="67"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="65"/>
@@ -4077,11 +4094,204 @@
       <c r="C98" s="93"/>
       <c r="D98" s="94">
         <f>SUM(D85:D92)-(D94+D96)</f>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="E98" s="93"/>
+    </row>
+    <row r="99" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="B101" s="91" t="s">
+        <v>65</v>
+      </c>
+      <c r="C101" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D101" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="E101" s="91" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="73">
+        <v>44638</v>
+      </c>
+      <c r="B102" s="74">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C102" s="74">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D102" s="74">
+        <f>SUM(C102-B102)</f>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E98" s="93"/>
-    </row>
-    <row r="99" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="E102" s="75"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="73"/>
+      <c r="B103" s="76">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C103" s="74">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D103" s="74">
+        <f t="shared" ref="D103:D109" si="12">SUM(C103-B103)</f>
+        <v>0</v>
+      </c>
+      <c r="E103" s="75"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="67"/>
+      <c r="B104" s="68">
+        <v>0.5</v>
+      </c>
+      <c r="C104" s="69">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D104" s="69">
+        <f t="shared" si="12"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E104" s="92" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="75"/>
+      <c r="B105" s="76">
+        <f t="shared" ref="B105:B109" si="13">C104</f>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C105" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D105" s="74">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="E105" s="75"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="75"/>
+      <c r="B106" s="76">
+        <f t="shared" si="13"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C106" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D106" s="74">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="E106" s="75"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="75"/>
+      <c r="B107" s="76">
+        <f t="shared" si="13"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C107" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D107" s="74">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="E107" s="75"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="75"/>
+      <c r="B108" s="76">
+        <f t="shared" si="13"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C108" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D108" s="74">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="E108" s="75"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="75"/>
+      <c r="B109" s="76">
+        <f t="shared" si="13"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C109" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D109" s="74">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="E109" s="75"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="86"/>
+      <c r="B110" s="87"/>
+      <c r="C110" s="87"/>
+      <c r="D110" s="88"/>
+      <c r="E110" s="86"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="B111" s="68"/>
+      <c r="C111" s="68"/>
+      <c r="D111" s="69">
+        <f>D104+D106+D107</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E111" s="67"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="65"/>
+      <c r="B112" s="66"/>
+      <c r="C112" s="66"/>
+      <c r="D112" s="64"/>
+      <c r="E112" s="65"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="79" t="s">
+        <v>85</v>
+      </c>
+      <c r="B113" s="80"/>
+      <c r="C113" s="80"/>
+      <c r="D113" s="78"/>
+      <c r="E113" s="79"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="65"/>
+      <c r="B114" s="66"/>
+      <c r="C114" s="66"/>
+      <c r="D114" s="64"/>
+      <c r="E114" s="65"/>
+    </row>
+    <row r="115" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="93" t="s">
+        <v>86</v>
+      </c>
+      <c r="B115" s="93"/>
+      <c r="C115" s="93"/>
+      <c r="D115" s="94">
+        <f>SUM(D102:D109)-(D111+D113)</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E115" s="93"/>
+    </row>
+    <row r="116" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
v0.030 fix init + print fixtures
</commit_message>
<xml_diff>
--- a/FBM-planning.xlsx
+++ b/FBM-planning.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="108">
   <si>
     <t>M</t>
   </si>
@@ -329,7 +329,19 @@
     <t>Huvudvärk</t>
   </si>
   <si>
-    <t>Unit testing with xUnit</t>
+    <t>Networking, LinkedIn, mails etc.</t>
+  </si>
+  <si>
+    <t>read up on Unit testing with xUnit</t>
+  </si>
+  <si>
+    <t>read up on Unit testing with xUnit (Pluralsight)</t>
+  </si>
+  <si>
+    <t>create new tests</t>
+  </si>
+  <si>
+    <t>Middag + vila</t>
   </si>
 </sst>
 </file>
@@ -643,7 +655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -757,6 +769,7 @@
     <xf numFmtId="165" fontId="0" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="18" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2893,10 +2906,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3922,272 +3935,289 @@
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="73">
+      <c r="A85" s="95">
         <v>44637</v>
       </c>
-      <c r="B85" s="74">
+      <c r="B85" s="78">
         <v>0.375</v>
       </c>
-      <c r="C85" s="74">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="D85" s="74">
+      <c r="C85" s="78">
+        <v>0.4375</v>
+      </c>
+      <c r="D85" s="78">
         <f>SUM(C85-B85)</f>
-        <v>4.1666666666666685E-2</v>
-      </c>
-      <c r="E85" s="75" t="s">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E85" s="97" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="73"/>
       <c r="B86" s="76">
-        <v>0.41666666666666669</v>
+        <f>C85</f>
+        <v>0.4375</v>
       </c>
       <c r="C86" s="74">
-        <v>0.41666666666666669</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="D86" s="74">
-        <f t="shared" ref="D86:D92" si="10">SUM(C86-B86)</f>
-        <v>0</v>
-      </c>
-      <c r="E86" s="75"/>
+        <f>SUM(C86-B86)</f>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="E86" s="75" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="67"/>
       <c r="B87" s="68">
-        <v>0.5</v>
+        <f>C86</f>
+        <v>0.47916666666666669</v>
       </c>
       <c r="C87" s="69">
         <v>0.54166666666666663</v>
       </c>
       <c r="D87" s="69">
-        <f t="shared" si="10"/>
-        <v>4.166666666666663E-2</v>
+        <f t="shared" ref="D87:D93" si="10">SUM(C87-B87)</f>
+        <v>6.2499999999999944E-2</v>
       </c>
       <c r="E87" s="92" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="75"/>
-      <c r="B88" s="76">
+      <c r="A88" s="79"/>
+      <c r="B88" s="80">
         <f t="shared" ref="B88:B92" si="11">C87</f>
         <v>0.54166666666666663</v>
       </c>
-      <c r="C88" s="74">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D88" s="74">
+      <c r="C88" s="78">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D88" s="78">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="E88" s="75"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E88" s="79" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="75"/>
       <c r="B89" s="76">
         <f t="shared" si="11"/>
-        <v>0.54166666666666663</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="C89" s="74">
-        <v>0.54166666666666663</v>
+        <v>0.6875</v>
       </c>
       <c r="D89" s="74">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="E89" s="75"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E89" s="75" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="75"/>
-      <c r="B90" s="76">
+      <c r="A90" s="67"/>
+      <c r="B90" s="68">
         <f t="shared" si="11"/>
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C90" s="74">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D90" s="74">
+        <v>0.6875</v>
+      </c>
+      <c r="C90" s="69">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D90" s="69">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="E90" s="75"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E90" s="67" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="75"/>
       <c r="B91" s="76">
         <f t="shared" si="11"/>
-        <v>0.54166666666666663</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="C91" s="74">
-        <v>0.54166666666666663</v>
+        <v>0.76041666666666663</v>
       </c>
       <c r="D91" s="74">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="E91" s="75"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E91" s="75" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="75"/>
-      <c r="B92" s="76">
+      <c r="A92" s="67"/>
+      <c r="B92" s="68">
         <f t="shared" si="11"/>
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C92" s="74">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D92" s="74">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="C92" s="69">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="D92" s="69">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="E92" s="75"/>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="E92" s="67" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="86"/>
-      <c r="B93" s="87"/>
-      <c r="C93" s="87"/>
-      <c r="D93" s="88"/>
-      <c r="E93" s="86"/>
+      <c r="A93" s="75"/>
+      <c r="B93" s="76">
+        <f t="shared" ref="B93" si="12">C92</f>
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="C93" s="74">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="D93" s="74">
+        <f t="shared" si="10"/>
+        <v>9.375E-2</v>
+      </c>
+      <c r="E93" s="75"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="67" t="s">
+      <c r="A94" s="86"/>
+      <c r="B94" s="87"/>
+      <c r="C94" s="87"/>
+      <c r="D94" s="88"/>
+      <c r="E94" s="86"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="B94" s="68"/>
-      <c r="C94" s="68"/>
-      <c r="D94" s="69">
-        <f>D87+D89+D90</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-      <c r="E94" s="67"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="65"/>
-      <c r="B95" s="66"/>
-      <c r="C95" s="66"/>
-      <c r="D95" s="64"/>
-      <c r="E95" s="65"/>
+      <c r="B95" s="68"/>
+      <c r="C95" s="68"/>
+      <c r="D95" s="69">
+        <f>D87+D90+D92</f>
+        <v>0.11458333333333331</v>
+      </c>
+      <c r="E95" s="67"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="79" t="s">
+      <c r="A96" s="65"/>
+      <c r="B96" s="66"/>
+      <c r="C96" s="66"/>
+      <c r="D96" s="64"/>
+      <c r="E96" s="65"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="B96" s="80"/>
-      <c r="C96" s="80"/>
-      <c r="D96" s="78"/>
-      <c r="E96" s="79"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="65"/>
-      <c r="B97" s="66"/>
-      <c r="C97" s="66"/>
-      <c r="D97" s="64"/>
-      <c r="E97" s="65"/>
-    </row>
-    <row r="98" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="93" t="s">
+      <c r="B97" s="80"/>
+      <c r="C97" s="80"/>
+      <c r="D97" s="78">
+        <f>SUM(D85+D88)</f>
+        <v>0.125</v>
+      </c>
+      <c r="E97" s="79"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="65"/>
+      <c r="B98" s="66"/>
+      <c r="C98" s="66"/>
+      <c r="D98" s="64"/>
+      <c r="E98" s="65"/>
+    </row>
+    <row r="99" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="93" t="s">
         <v>86</v>
       </c>
-      <c r="B98" s="93"/>
-      <c r="C98" s="93"/>
-      <c r="D98" s="94">
-        <f>SUM(D85:D92)-(D94+D96)</f>
-        <v>4.1666666666666685E-2</v>
-      </c>
-      <c r="E98" s="93"/>
-    </row>
-    <row r="99" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="91" t="s">
+      <c r="B99" s="93"/>
+      <c r="C99" s="93"/>
+      <c r="D99" s="94">
+        <f>SUM(D85:D93)-(D95+D97)</f>
+        <v>0.28125000000000006</v>
+      </c>
+      <c r="E99" s="93"/>
+    </row>
+    <row r="100" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="B101" s="91" t="s">
+      <c r="B102" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="C101" s="91" t="s">
+      <c r="C102" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="D101" s="91" t="s">
+      <c r="D102" s="91" t="s">
         <v>68</v>
       </c>
-      <c r="E101" s="91" t="s">
+      <c r="E102" s="91" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="73">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="73">
         <v>44638</v>
       </c>
-      <c r="B102" s="74">
+      <c r="B103" s="74">
         <v>0.33333333333333331</v>
-      </c>
-      <c r="C102" s="74">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="D102" s="74">
-        <f>SUM(C102-B102)</f>
-        <v>8.333333333333337E-2</v>
-      </c>
-      <c r="E102" s="75"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="73"/>
-      <c r="B103" s="76">
-        <v>0.41666666666666669</v>
       </c>
       <c r="C103" s="74">
         <v>0.41666666666666669</v>
       </c>
       <c r="D103" s="74">
-        <f t="shared" ref="D103:D109" si="12">SUM(C103-B103)</f>
+        <f>SUM(C103-B103)</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E103" s="75"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="73"/>
+      <c r="B104" s="76">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C104" s="74">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D104" s="74">
+        <f t="shared" ref="D104:D110" si="13">SUM(C104-B104)</f>
         <v>0</v>
       </c>
-      <c r="E103" s="75"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="67"/>
-      <c r="B104" s="68">
+      <c r="E104" s="75"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="67"/>
+      <c r="B105" s="68">
         <v>0.5</v>
       </c>
-      <c r="C104" s="69">
+      <c r="C105" s="69">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D104" s="69">
-        <f t="shared" si="12"/>
+      <c r="D105" s="69">
+        <f t="shared" si="13"/>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="E104" s="92" t="s">
+      <c r="E105" s="92" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="75"/>
-      <c r="B105" s="76">
-        <f t="shared" ref="B105:B109" si="13">C104</f>
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C105" s="74">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D105" s="74">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="E105" s="75"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="75"/>
       <c r="B106" s="76">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="B106:B110" si="14">C105</f>
         <v>0.54166666666666663</v>
       </c>
       <c r="C106" s="74">
         <v>0.54166666666666663</v>
       </c>
       <c r="D106" s="74">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="E106" s="75"/>
@@ -4195,14 +4225,14 @@
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="75"/>
       <c r="B107" s="76">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.54166666666666663</v>
       </c>
       <c r="C107" s="74">
         <v>0.54166666666666663</v>
       </c>
       <c r="D107" s="74">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="E107" s="75"/>
@@ -4210,14 +4240,14 @@
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="75"/>
       <c r="B108" s="76">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.54166666666666663</v>
       </c>
       <c r="C108" s="74">
         <v>0.54166666666666663</v>
       </c>
       <c r="D108" s="74">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="E108" s="75"/>
@@ -4225,73 +4255,88 @@
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="75"/>
       <c r="B109" s="76">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.54166666666666663</v>
       </c>
       <c r="C109" s="74">
         <v>0.54166666666666663</v>
       </c>
       <c r="D109" s="74">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="E109" s="75"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="86"/>
-      <c r="B110" s="87"/>
-      <c r="C110" s="87"/>
-      <c r="D110" s="88"/>
-      <c r="E110" s="86"/>
+      <c r="A110" s="75"/>
+      <c r="B110" s="76">
+        <f t="shared" si="14"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C110" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D110" s="74">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="E110" s="75"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="67" t="s">
+      <c r="A111" s="86"/>
+      <c r="B111" s="87"/>
+      <c r="C111" s="87"/>
+      <c r="D111" s="88"/>
+      <c r="E111" s="86"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="B111" s="68"/>
-      <c r="C111" s="68"/>
-      <c r="D111" s="69">
-        <f>D104+D106+D107</f>
+      <c r="B112" s="68"/>
+      <c r="C112" s="68"/>
+      <c r="D112" s="69">
+        <f>D105+D107+D108</f>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="E111" s="67"/>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="65"/>
-      <c r="B112" s="66"/>
-      <c r="C112" s="66"/>
-      <c r="D112" s="64"/>
-      <c r="E112" s="65"/>
+      <c r="E112" s="67"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="79" t="s">
+      <c r="A113" s="65"/>
+      <c r="B113" s="66"/>
+      <c r="C113" s="66"/>
+      <c r="D113" s="64"/>
+      <c r="E113" s="65"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="B113" s="80"/>
-      <c r="C113" s="80"/>
-      <c r="D113" s="78"/>
-      <c r="E113" s="79"/>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="65"/>
-      <c r="B114" s="66"/>
-      <c r="C114" s="66"/>
-      <c r="D114" s="64"/>
-      <c r="E114" s="65"/>
-    </row>
-    <row r="115" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="93" t="s">
+      <c r="B114" s="80"/>
+      <c r="C114" s="80"/>
+      <c r="D114" s="78"/>
+      <c r="E114" s="79"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="65"/>
+      <c r="B115" s="66"/>
+      <c r="C115" s="66"/>
+      <c r="D115" s="64"/>
+      <c r="E115" s="65"/>
+    </row>
+    <row r="116" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="93" t="s">
         <v>86</v>
       </c>
-      <c r="B115" s="93"/>
-      <c r="C115" s="93"/>
-      <c r="D115" s="94">
-        <f>SUM(D102:D109)-(D111+D113)</f>
+      <c r="B116" s="93"/>
+      <c r="C116" s="93"/>
+      <c r="D116" s="94">
+        <f>SUM(D103:D110)-(D112+D114)</f>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E115" s="93"/>
-    </row>
-    <row r="116" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="E116" s="93"/>
+    </row>
+    <row r="117" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
v0.033 GetNextFixture, DeleteFixture, PrintFixture, PrintFixtures
</commit_message>
<xml_diff>
--- a/FBM-planning.xlsx
+++ b/FBM-planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18960" windowHeight="12045" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18960" windowHeight="12045" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feb" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="123">
   <si>
     <t>M</t>
   </si>
@@ -342,6 +342,51 @@
   </si>
   <si>
     <t>Middag + vila</t>
+  </si>
+  <si>
+    <t>tutorial xUnit unit tests</t>
+  </si>
+  <si>
+    <t>Jobbsökaraktiviteter</t>
+  </si>
+  <si>
+    <t>skicka ansökan Ammi, lägga in i AF portalen</t>
+  </si>
+  <si>
+    <t>fix Todo items for Task List</t>
+  </si>
+  <si>
+    <t>Jobbsökaraktiviteter, sökt jobb Ammi tech AB</t>
+  </si>
+  <si>
+    <t>Update Fixture</t>
+  </si>
+  <si>
+    <t>Problem with Delete Fixture</t>
+  </si>
+  <si>
+    <t>Vindskivor</t>
+  </si>
+  <si>
+    <t>Delete Fixtures</t>
+  </si>
+  <si>
+    <t>Create Fixture</t>
+  </si>
+  <si>
+    <t>Fix Fixture Delete FixtureDeleteHandler</t>
+  </si>
+  <si>
+    <t>fix GetNextFixture</t>
+  </si>
+  <si>
+    <t>Init Fixtures/Print Fixtures to Console</t>
+  </si>
+  <si>
+    <t>NextMatchDay passed into GetMatchDay method</t>
+  </si>
+  <si>
+    <t>GetNextFixture</t>
   </si>
 </sst>
 </file>
@@ -384,7 +429,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -514,6 +559,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -655,7 +706,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -770,6 +821,8 @@
     <xf numFmtId="16" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="18" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2082,16 +2135,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH31"/>
+  <dimension ref="A1:AH37"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N31" sqref="N31"/>
+      <selection pane="topRight" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="32" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2114,6 +2167,13 @@
       <c r="G1">
         <v>8</v>
       </c>
+      <c r="H1" s="98" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
       <c r="AH1">
         <f>SUM(B1:AF1)</f>
         <v>40</v>
@@ -2307,8 +2367,8 @@
       <c r="A4" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
@@ -2345,7 +2405,7 @@
         <v>33</v>
       </c>
       <c r="N11" s="40"/>
-      <c r="O11" s="40"/>
+      <c r="T11" s="40"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
@@ -2431,28 +2491,28 @@
         <v>20</v>
       </c>
       <c r="N22" s="41"/>
-      <c r="O22" s="41"/>
+      <c r="U22" s="41"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>22</v>
       </c>
       <c r="N23" s="41"/>
-      <c r="O23" s="41"/>
+      <c r="U23" s="41"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="O24" s="41"/>
-      <c r="P24" s="41"/>
+      <c r="U24" s="41"/>
+      <c r="V24" s="41"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="O25" s="41"/>
-      <c r="P25" s="41"/>
+      <c r="U25" s="41"/>
+      <c r="V25" s="41"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
@@ -2467,33 +2527,80 @@
       </c>
       <c r="G27" s="37"/>
       <c r="N27" s="37"/>
-      <c r="O27" s="41"/>
+      <c r="U27" s="23"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
         <v>77</v>
       </c>
       <c r="N28" s="37"/>
-      <c r="O28" s="41"/>
+      <c r="U28" s="41"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>78</v>
       </c>
       <c r="N29" s="23"/>
-      <c r="O29" s="41"/>
+      <c r="O29" s="37"/>
+      <c r="U29" s="41"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="O30" s="41"/>
+      <c r="O30" s="37"/>
+      <c r="U30" s="41"/>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>80</v>
       </c>
       <c r="N31" s="37"/>
+      <c r="O31" s="37"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="O32" s="23"/>
+      <c r="P32" s="37"/>
+      <c r="Q32" s="37"/>
+      <c r="R32" s="37"/>
+      <c r="S32" s="37"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="O33" s="23"/>
+      <c r="P33" s="37"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="O34" s="23"/>
+      <c r="P34" s="37"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q35" s="37"/>
+      <c r="R35" s="37"/>
+      <c r="S35" s="37"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="T36" s="37"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="T37" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2906,10 +3013,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E117"/>
+  <dimension ref="A1:G137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="E124" sqref="E124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4112,7 +4219,7 @@
       <c r="D96" s="64"/>
       <c r="E96" s="65"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="79" t="s">
         <v>85</v>
       </c>
@@ -4124,14 +4231,14 @@
       </c>
       <c r="E97" s="79"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="65"/>
       <c r="B98" s="66"/>
       <c r="C98" s="66"/>
       <c r="D98" s="64"/>
       <c r="E98" s="65"/>
     </row>
-    <row r="99" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="93" t="s">
         <v>86</v>
       </c>
@@ -4143,8 +4250,8 @@
       </c>
       <c r="E99" s="93"/>
     </row>
-    <row r="100" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="91" t="s">
         <v>64</v>
       </c>
@@ -4161,182 +4268,452 @@
         <v>67</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="73">
         <v>44638</v>
       </c>
       <c r="B103" s="74">
-        <v>0.33333333333333331</v>
+        <v>0.42708333333333331</v>
       </c>
       <c r="C103" s="74">
-        <v>0.41666666666666669</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="D103" s="74">
         <f>SUM(C103-B103)</f>
-        <v>8.333333333333337E-2</v>
-      </c>
-      <c r="E103" s="75"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="73"/>
-      <c r="B104" s="76">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="C104" s="74">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="D104" s="74">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E103" s="75" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="95"/>
+      <c r="B104" s="80">
+        <f>C103</f>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C104" s="78">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D104" s="78">
         <f t="shared" ref="D104:D110" si="13">SUM(C104-B104)</f>
-        <v>0</v>
-      </c>
-      <c r="E104" s="75"/>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E104" s="79" t="s">
+        <v>109</v>
+      </c>
+      <c r="G104" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="67"/>
       <c r="B105" s="68">
-        <v>0.5</v>
+        <f>C104</f>
+        <v>0.47916666666666669</v>
       </c>
       <c r="C105" s="69">
-        <v>0.54166666666666663</v>
+        <v>0.53125</v>
       </c>
       <c r="D105" s="69">
         <f t="shared" si="13"/>
-        <v>4.166666666666663E-2</v>
+        <v>5.2083333333333315E-2</v>
       </c>
       <c r="E105" s="92" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="75"/>
       <c r="B106" s="76">
         <f t="shared" ref="B106:B110" si="14">C105</f>
-        <v>0.54166666666666663</v>
+        <v>0.53125</v>
       </c>
       <c r="C106" s="74">
         <v>0.54166666666666663</v>
       </c>
       <c r="D106" s="74">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="E106" s="75"/>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E106" s="75" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="75"/>
       <c r="B107" s="76">
         <f t="shared" si="14"/>
         <v>0.54166666666666663</v>
       </c>
       <c r="C107" s="74">
-        <v>0.54166666666666663</v>
+        <v>0.5625</v>
       </c>
       <c r="D107" s="74">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="E107" s="75"/>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="75"/>
-      <c r="B108" s="76">
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E107" s="75" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="79"/>
+      <c r="B108" s="80">
         <f t="shared" si="14"/>
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C108" s="74">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D108" s="74">
+        <v>0.5625</v>
+      </c>
+      <c r="C108" s="78">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D108" s="78">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="E108" s="75"/>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E108" s="79" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="75"/>
       <c r="B109" s="76">
         <f t="shared" si="14"/>
-        <v>0.54166666666666663</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="C109" s="74">
-        <v>0.54166666666666663</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="D109" s="74">
         <f t="shared" si="13"/>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="E109" s="75" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="67"/>
+      <c r="B110" s="68">
+        <f t="shared" si="14"/>
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C110" s="69">
+        <v>0.65625</v>
+      </c>
+      <c r="D110" s="69">
+        <f t="shared" si="13"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E110" s="67" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="75"/>
+      <c r="B111" s="76">
+        <f t="shared" ref="B111" si="15">C110</f>
+        <v>0.65625</v>
+      </c>
+      <c r="C111" s="74">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D111" s="74">
+        <f>SUM(C111-B111)</f>
+        <v>7.291666666666663E-2</v>
+      </c>
+      <c r="E111" s="75" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="86"/>
+      <c r="B112" s="87"/>
+      <c r="C112" s="87"/>
+      <c r="D112" s="88"/>
+      <c r="E112" s="86"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="B113" s="68"/>
+      <c r="C113" s="68"/>
+      <c r="D113" s="69">
+        <f>D105+D110</f>
+        <v>6.2499999999999944E-2</v>
+      </c>
+      <c r="E113" s="67"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="65"/>
+      <c r="B114" s="66"/>
+      <c r="C114" s="66"/>
+      <c r="D114" s="64"/>
+      <c r="E114" s="65"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="79" t="s">
+        <v>85</v>
+      </c>
+      <c r="B115" s="80"/>
+      <c r="C115" s="80"/>
+      <c r="D115" s="78">
+        <f>D104+D108</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E115" s="79"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="65"/>
+      <c r="B116" s="66"/>
+      <c r="C116" s="66"/>
+      <c r="D116" s="64"/>
+      <c r="E116" s="65"/>
+    </row>
+    <row r="117" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="93" t="s">
+        <v>86</v>
+      </c>
+      <c r="B117" s="93"/>
+      <c r="C117" s="93"/>
+      <c r="D117" s="94">
+        <f>SUM(D103:D111)-(D113+D115)</f>
+        <v>0.17708333333333337</v>
+      </c>
+      <c r="E117" s="93"/>
+    </row>
+    <row r="118" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="B120" s="91" t="s">
+        <v>65</v>
+      </c>
+      <c r="C120" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D120" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="E120" s="91" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="73">
+        <v>44639</v>
+      </c>
+      <c r="B121" s="74">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C121" s="74">
+        <v>0.40625</v>
+      </c>
+      <c r="D121" s="74">
+        <f>SUM(C121-B121)</f>
+        <v>5.2083333333333315E-2</v>
+      </c>
+      <c r="E121" s="75" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="96"/>
+      <c r="B122" s="68">
+        <f>C121</f>
+        <v>0.40625</v>
+      </c>
+      <c r="C122" s="69">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D122" s="69">
+        <f>SUM(C122-B122)</f>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="E122" s="67" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="73"/>
+      <c r="B123" s="76">
+        <f>C122</f>
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="C123" s="74">
+        <v>0.5</v>
+      </c>
+      <c r="D123" s="74">
+        <f>SUM(C123-B123)</f>
+        <v>6.944444444444442E-2</v>
+      </c>
+      <c r="E123" s="99" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="67"/>
+      <c r="B124" s="68">
+        <f>C123</f>
+        <v>0.5</v>
+      </c>
+      <c r="C124" s="69">
+        <v>0.5</v>
+      </c>
+      <c r="D124" s="69">
+        <f t="shared" ref="D123:D129" si="16">SUM(C124-B124)</f>
         <v>0</v>
       </c>
-      <c r="E109" s="75"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="75"/>
-      <c r="B110" s="76">
-        <f t="shared" si="14"/>
+      <c r="E124" s="92" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="75"/>
+      <c r="B125" s="76">
+        <f t="shared" ref="B125:B130" si="17">C124</f>
+        <v>0.5</v>
+      </c>
+      <c r="C125" s="74">
         <v>0.54166666666666663</v>
       </c>
-      <c r="C110" s="74">
+      <c r="D125" s="74">
+        <f t="shared" si="16"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E125" s="75"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="75"/>
+      <c r="B126" s="76">
+        <f t="shared" si="17"/>
         <v>0.54166666666666663</v>
       </c>
-      <c r="D110" s="74">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="E110" s="75"/>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="86"/>
-      <c r="B111" s="87"/>
-      <c r="C111" s="87"/>
-      <c r="D111" s="88"/>
-      <c r="E111" s="86"/>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="67" t="s">
+      <c r="C126" s="74">
+        <v>0.5625</v>
+      </c>
+      <c r="D126" s="74">
+        <f t="shared" si="16"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E126" s="75"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="75"/>
+      <c r="B127" s="76">
+        <f t="shared" si="17"/>
+        <v>0.5625</v>
+      </c>
+      <c r="C127" s="74">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D127" s="74">
+        <f t="shared" si="16"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E127" s="75"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="75"/>
+      <c r="B128" s="76">
+        <f t="shared" si="17"/>
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C128" s="74">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D128" s="74">
+        <f t="shared" si="16"/>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="E128" s="75"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="75"/>
+      <c r="B129" s="76">
+        <f t="shared" si="17"/>
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C129" s="74">
+        <v>0.65625</v>
+      </c>
+      <c r="D129" s="74">
+        <f t="shared" si="16"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E129" s="75"/>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="75"/>
+      <c r="B130" s="76">
+        <f t="shared" si="17"/>
+        <v>0.65625</v>
+      </c>
+      <c r="C130" s="74">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D130" s="74">
+        <f>SUM(C130-B130)</f>
+        <v>7.291666666666663E-2</v>
+      </c>
+      <c r="E130" s="75"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="75"/>
+      <c r="B131" s="76"/>
+      <c r="C131" s="76"/>
+      <c r="D131" s="74"/>
+      <c r="E131" s="75"/>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="B112" s="68"/>
-      <c r="C112" s="68"/>
-      <c r="D112" s="69">
-        <f>D105+D107+D108</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-      <c r="E112" s="67"/>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="65"/>
-      <c r="B113" s="66"/>
-      <c r="C113" s="66"/>
-      <c r="D113" s="64"/>
-      <c r="E113" s="65"/>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="79" t="s">
+      <c r="B132" s="68"/>
+      <c r="C132" s="68"/>
+      <c r="D132" s="69">
+        <f>D122+D124</f>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="E132" s="67"/>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="65"/>
+      <c r="B133" s="66"/>
+      <c r="C133" s="66"/>
+      <c r="D133" s="64"/>
+      <c r="E133" s="65"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="B114" s="80"/>
-      <c r="C114" s="80"/>
-      <c r="D114" s="78"/>
-      <c r="E114" s="79"/>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="65"/>
-      <c r="B115" s="66"/>
-      <c r="C115" s="66"/>
-      <c r="D115" s="64"/>
-      <c r="E115" s="65"/>
-    </row>
-    <row r="116" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="93" t="s">
+      <c r="B134" s="80"/>
+      <c r="C134" s="80"/>
+      <c r="D134" s="78"/>
+      <c r="E134" s="79"/>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="65"/>
+      <c r="B135" s="66"/>
+      <c r="C135" s="66"/>
+      <c r="D135" s="64"/>
+      <c r="E135" s="65"/>
+    </row>
+    <row r="136" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="93" t="s">
         <v>86</v>
       </c>
-      <c r="B116" s="93"/>
-      <c r="C116" s="93"/>
-      <c r="D116" s="94">
-        <f>SUM(D103:D110)-(D112+D114)</f>
-        <v>8.333333333333337E-2</v>
-      </c>
-      <c r="E116" s="93"/>
-    </row>
-    <row r="117" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="B136" s="93"/>
+      <c r="C136" s="93"/>
+      <c r="D136" s="94">
+        <f>SUM(D121:D130)-(D132+D134)</f>
+        <v>0.35069444444444436</v>
+      </c>
+      <c r="E136" s="93"/>
+    </row>
+    <row r="137" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
v0.037 InitManagedTeamPlayers w 10 plyrs, PrintManagedTeam
</commit_message>
<xml_diff>
--- a/FBM-planning.xlsx
+++ b/FBM-planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18960" windowHeight="12045" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18960" windowHeight="12045" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Feb" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="126">
   <si>
     <t>M</t>
   </si>
@@ -387,6 +387,15 @@
   </si>
   <si>
     <t>GetNextFixture</t>
+  </si>
+  <si>
+    <t>fix projects folder structure</t>
+  </si>
+  <si>
+    <t>PrintTeamPlayers, Navigation</t>
+  </si>
+  <si>
+    <t>Veterinären</t>
   </si>
 </sst>
 </file>
@@ -706,7 +715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -823,6 +832,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2137,7 +2148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A36" sqref="A36"/>
     </sheetView>
@@ -3013,10 +3024,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G137"/>
+  <dimension ref="A1:G181"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="E124" sqref="E124"/>
+    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="C169" sqref="C169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4553,167 +4564,522 @@
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" s="67"/>
-      <c r="B124" s="68">
-        <f>C123</f>
+      <c r="A124" s="100"/>
+      <c r="B124" s="87"/>
+      <c r="C124" s="88"/>
+      <c r="D124" s="88"/>
+      <c r="E124" s="23"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="B125" s="68"/>
+      <c r="C125" s="68"/>
+      <c r="D125" s="69">
+        <f>D122</f>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="E125" s="67"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="65"/>
+      <c r="B126" s="66"/>
+      <c r="C126" s="66"/>
+      <c r="D126" s="64"/>
+      <c r="E126" s="65"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="79" t="s">
+        <v>85</v>
+      </c>
+      <c r="B127" s="80"/>
+      <c r="C127" s="80"/>
+      <c r="D127" s="78"/>
+      <c r="E127" s="79"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="65"/>
+      <c r="B128" s="66"/>
+      <c r="C128" s="66"/>
+      <c r="D128" s="64"/>
+      <c r="E128" s="65"/>
+    </row>
+    <row r="129" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="93" t="s">
+        <v>86</v>
+      </c>
+      <c r="B129" s="93"/>
+      <c r="C129" s="93"/>
+      <c r="D129" s="94">
+        <f>SUM(D121:D123)-(D125+D127)</f>
+        <v>0.12152777777777773</v>
+      </c>
+      <c r="E129" s="93"/>
+    </row>
+    <row r="130" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="B132" s="91" t="s">
+        <v>65</v>
+      </c>
+      <c r="C132" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D132" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="E132" s="91" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="73">
+        <v>44640</v>
+      </c>
+      <c r="B133" s="74">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C133" s="74">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D133" s="74">
+        <f>SUM(C133-B133)</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E133" s="75" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="96"/>
+      <c r="B134" s="68">
+        <f>C133</f>
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C134" s="69">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="D134" s="69">
+        <f>SUM(C134-B134)</f>
+        <v>0.28124999999999994</v>
+      </c>
+      <c r="E134" s="67" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="73"/>
+      <c r="B135" s="76">
+        <f>C134</f>
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="C135" s="74">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D135" s="74">
+        <f>SUM(C135-B135)</f>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="E135" s="75" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="75"/>
+      <c r="B136" s="76">
+        <f>C135</f>
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C136" s="74">
+        <v>0.875</v>
+      </c>
+      <c r="D136" s="74">
+        <f t="shared" ref="D136" si="16">SUM(C136-B136)</f>
+        <v>0.10416666666666663</v>
+      </c>
+      <c r="E136" s="101" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="75"/>
+      <c r="B137" s="76"/>
+      <c r="C137" s="74"/>
+      <c r="D137" s="74"/>
+      <c r="E137" s="75"/>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="75"/>
+      <c r="B138" s="76"/>
+      <c r="C138" s="74"/>
+      <c r="D138" s="74"/>
+      <c r="E138" s="75"/>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="75"/>
+      <c r="B139" s="76"/>
+      <c r="C139" s="74"/>
+      <c r="D139" s="74"/>
+      <c r="E139" s="75"/>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="75"/>
+      <c r="B140" s="76"/>
+      <c r="C140" s="74"/>
+      <c r="D140" s="74"/>
+      <c r="E140" s="75"/>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="75"/>
+      <c r="B141" s="76"/>
+      <c r="C141" s="74"/>
+      <c r="D141" s="74"/>
+      <c r="E141" s="75"/>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="75"/>
+      <c r="B142" s="76"/>
+      <c r="C142" s="74"/>
+      <c r="D142" s="74"/>
+      <c r="E142" s="75"/>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="75"/>
+      <c r="B143" s="76"/>
+      <c r="C143" s="76"/>
+      <c r="D143" s="74"/>
+      <c r="E143" s="75"/>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="B144" s="68"/>
+      <c r="C144" s="68"/>
+      <c r="D144" s="69">
+        <f>D134</f>
+        <v>0.28124999999999994</v>
+      </c>
+      <c r="E144" s="67"/>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="65"/>
+      <c r="B145" s="66"/>
+      <c r="C145" s="66"/>
+      <c r="D145" s="64"/>
+      <c r="E145" s="65"/>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="79" t="s">
+        <v>85</v>
+      </c>
+      <c r="B146" s="80"/>
+      <c r="C146" s="80"/>
+      <c r="D146" s="78"/>
+      <c r="E146" s="79"/>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="65"/>
+      <c r="B147" s="66"/>
+      <c r="C147" s="66"/>
+      <c r="D147" s="64"/>
+      <c r="E147" s="65"/>
+    </row>
+    <row r="148" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="93" t="s">
+        <v>86</v>
+      </c>
+      <c r="B148" s="93"/>
+      <c r="C148" s="93"/>
+      <c r="D148" s="94">
+        <f>SUM(D133:D142)-(D144+D146)</f>
+        <v>0.17708333333333337</v>
+      </c>
+      <c r="E148" s="93"/>
+    </row>
+    <row r="149" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="B151" s="91" t="s">
+        <v>65</v>
+      </c>
+      <c r="C151" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D151" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="E151" s="91" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="73">
+        <v>44641</v>
+      </c>
+      <c r="B152" s="74"/>
+      <c r="C152" s="74"/>
+      <c r="D152" s="74"/>
+      <c r="E152" s="75"/>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="96"/>
+      <c r="B153" s="68"/>
+      <c r="C153" s="69"/>
+      <c r="D153" s="69"/>
+      <c r="E153" s="67" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="73"/>
+      <c r="B154" s="76"/>
+      <c r="C154" s="74"/>
+      <c r="D154" s="74"/>
+      <c r="E154" s="75"/>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="75"/>
+      <c r="B155" s="76"/>
+      <c r="C155" s="74"/>
+      <c r="D155" s="74"/>
+      <c r="E155" s="101"/>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="75"/>
+      <c r="B156" s="76"/>
+      <c r="C156" s="76"/>
+      <c r="D156" s="74"/>
+      <c r="E156" s="75"/>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="B157" s="68"/>
+      <c r="C157" s="68"/>
+      <c r="D157" s="69">
+        <f>D153</f>
+        <v>0</v>
+      </c>
+      <c r="E157" s="67"/>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="65"/>
+      <c r="B158" s="66"/>
+      <c r="C158" s="66"/>
+      <c r="D158" s="64"/>
+      <c r="E158" s="65"/>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="79" t="s">
+        <v>85</v>
+      </c>
+      <c r="B159" s="80"/>
+      <c r="C159" s="80"/>
+      <c r="D159" s="78"/>
+      <c r="E159" s="79"/>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="65"/>
+      <c r="B160" s="66"/>
+      <c r="C160" s="66"/>
+      <c r="D160" s="64"/>
+      <c r="E160" s="65"/>
+    </row>
+    <row r="161" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="93" t="s">
+        <v>86</v>
+      </c>
+      <c r="B161" s="93"/>
+      <c r="C161" s="93"/>
+      <c r="D161" s="94">
+        <f>SUM(D152:D155)-(D157+D159)</f>
+        <v>0</v>
+      </c>
+      <c r="E161" s="93"/>
+    </row>
+    <row r="162" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="B164" s="91" t="s">
+        <v>65</v>
+      </c>
+      <c r="C164" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D164" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="E164" s="91" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="73">
+        <v>44642</v>
+      </c>
+      <c r="B165" s="74">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="C165" s="74">
         <v>0.5</v>
       </c>
-      <c r="C124" s="69">
+      <c r="D165" s="74">
+        <f>SUM(C165-B165)</f>
+        <v>5.2083333333333315E-2</v>
+      </c>
+      <c r="E165" s="75"/>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="96"/>
+      <c r="B166" s="68">
+        <f>C165</f>
         <v>0.5</v>
       </c>
-      <c r="D124" s="69">
-        <f t="shared" ref="D123:D129" si="16">SUM(C124-B124)</f>
+      <c r="C166" s="69">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="D166" s="69">
+        <f>SUM(C166-B166)</f>
+        <v>0.26041666666666663</v>
+      </c>
+      <c r="E166" s="67"/>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="73"/>
+      <c r="B167" s="76">
+        <f>C166</f>
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="C167" s="74">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D167" s="74">
+        <f>SUM(C167-B167)</f>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="E167" s="75"/>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="75"/>
+      <c r="B168" s="76">
+        <f>C167</f>
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C168" s="74">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D168" s="74">
+        <f t="shared" ref="D168" si="17">SUM(C168-B168)</f>
         <v>0</v>
       </c>
-      <c r="E124" s="92" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" s="75"/>
-      <c r="B125" s="76">
-        <f t="shared" ref="B125:B130" si="17">C124</f>
-        <v>0.5</v>
-      </c>
-      <c r="C125" s="74">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D125" s="74">
-        <f t="shared" si="16"/>
-        <v>4.166666666666663E-2</v>
-      </c>
-      <c r="E125" s="75"/>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="75"/>
-      <c r="B126" s="76">
-        <f t="shared" si="17"/>
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C126" s="74">
-        <v>0.5625</v>
-      </c>
-      <c r="D126" s="74">
-        <f t="shared" si="16"/>
-        <v>2.083333333333337E-2</v>
-      </c>
-      <c r="E126" s="75"/>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" s="75"/>
-      <c r="B127" s="76">
-        <f t="shared" si="17"/>
-        <v>0.5625</v>
-      </c>
-      <c r="C127" s="74">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="D127" s="74">
-        <f t="shared" si="16"/>
-        <v>4.166666666666663E-2</v>
-      </c>
-      <c r="E127" s="75"/>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" s="75"/>
-      <c r="B128" s="76">
-        <f t="shared" si="17"/>
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="C128" s="74">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="D128" s="74">
-        <f t="shared" si="16"/>
-        <v>4.1666666666666741E-2</v>
-      </c>
-      <c r="E128" s="75"/>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" s="75"/>
-      <c r="B129" s="76">
-        <f t="shared" si="17"/>
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="C129" s="74">
-        <v>0.65625</v>
-      </c>
-      <c r="D129" s="74">
-        <f t="shared" si="16"/>
-        <v>1.041666666666663E-2</v>
-      </c>
-      <c r="E129" s="75"/>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" s="75"/>
-      <c r="B130" s="76">
-        <f t="shared" si="17"/>
-        <v>0.65625</v>
-      </c>
-      <c r="C130" s="74">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="D130" s="74">
-        <f>SUM(C130-B130)</f>
-        <v>7.291666666666663E-2</v>
-      </c>
-      <c r="E130" s="75"/>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A131" s="75"/>
-      <c r="B131" s="76"/>
-      <c r="C131" s="76"/>
-      <c r="D131" s="74"/>
-      <c r="E131" s="75"/>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" s="67" t="s">
+      <c r="E168" s="101"/>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="75"/>
+      <c r="B169" s="76"/>
+      <c r="C169" s="74"/>
+      <c r="D169" s="74"/>
+      <c r="E169" s="75"/>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="75"/>
+      <c r="B170" s="76"/>
+      <c r="C170" s="74"/>
+      <c r="D170" s="74"/>
+      <c r="E170" s="75"/>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="75"/>
+      <c r="B171" s="76"/>
+      <c r="C171" s="74"/>
+      <c r="D171" s="74"/>
+      <c r="E171" s="75"/>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="75"/>
+      <c r="B172" s="76"/>
+      <c r="C172" s="74"/>
+      <c r="D172" s="74"/>
+      <c r="E172" s="75"/>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="75"/>
+      <c r="B173" s="76"/>
+      <c r="C173" s="74"/>
+      <c r="D173" s="74"/>
+      <c r="E173" s="75"/>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="75"/>
+      <c r="B174" s="76"/>
+      <c r="C174" s="74"/>
+      <c r="D174" s="74"/>
+      <c r="E174" s="75"/>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="75"/>
+      <c r="B175" s="76"/>
+      <c r="C175" s="76"/>
+      <c r="D175" s="74"/>
+      <c r="E175" s="75"/>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="B132" s="68"/>
-      <c r="C132" s="68"/>
-      <c r="D132" s="69">
-        <f>D122+D124</f>
-        <v>2.430555555555558E-2</v>
-      </c>
-      <c r="E132" s="67"/>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" s="65"/>
-      <c r="B133" s="66"/>
-      <c r="C133" s="66"/>
-      <c r="D133" s="64"/>
-      <c r="E133" s="65"/>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" s="79" t="s">
+      <c r="B176" s="68"/>
+      <c r="C176" s="68"/>
+      <c r="D176" s="69">
+        <f>D166</f>
+        <v>0.26041666666666663</v>
+      </c>
+      <c r="E176" s="67"/>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="65"/>
+      <c r="B177" s="66"/>
+      <c r="C177" s="66"/>
+      <c r="D177" s="64"/>
+      <c r="E177" s="65"/>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="B134" s="80"/>
-      <c r="C134" s="80"/>
-      <c r="D134" s="78"/>
-      <c r="E134" s="79"/>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" s="65"/>
-      <c r="B135" s="66"/>
-      <c r="C135" s="66"/>
-      <c r="D135" s="64"/>
-      <c r="E135" s="65"/>
-    </row>
-    <row r="136" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="93" t="s">
+      <c r="B178" s="80"/>
+      <c r="C178" s="80"/>
+      <c r="D178" s="78"/>
+      <c r="E178" s="79"/>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="65"/>
+      <c r="B179" s="66"/>
+      <c r="C179" s="66"/>
+      <c r="D179" s="64"/>
+      <c r="E179" s="65"/>
+    </row>
+    <row r="180" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A180" s="93" t="s">
         <v>86</v>
       </c>
-      <c r="B136" s="93"/>
-      <c r="C136" s="93"/>
-      <c r="D136" s="94">
-        <f>SUM(D121:D130)-(D132+D134)</f>
-        <v>0.35069444444444436</v>
-      </c>
-      <c r="E136" s="93"/>
-    </row>
-    <row r="137" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="B180" s="93"/>
+      <c r="C180" s="93"/>
+      <c r="D180" s="94">
+        <f>SUM(D165:D174)-(D176+D178)</f>
+        <v>6.2500000000000056E-2</v>
+      </c>
+      <c r="E180" s="93"/>
+    </row>
+    <row r="181" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
v0.038 delete player doubles, fix PlayerInit, PlayerUpdateCommand
</commit_message>
<xml_diff>
--- a/FBM-planning.xlsx
+++ b/FBM-planning.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="129">
   <si>
     <t>M</t>
   </si>
@@ -396,6 +396,15 @@
   </si>
   <si>
     <t>Veterinären</t>
+  </si>
+  <si>
+    <t>Lunch, veterinär mm</t>
+  </si>
+  <si>
+    <t>Init players</t>
+  </si>
+  <si>
+    <t>InitPlayers setup team with 10 players works</t>
   </si>
 </sst>
 </file>
@@ -715,7 +724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -834,6 +843,7 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3027,7 +3037,7 @@
   <dimension ref="A1:G181"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="C169" sqref="C169"/>
+      <selection activeCell="C172" sqref="C172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4936,7 +4946,9 @@
         <f>SUM(C165-B165)</f>
         <v>5.2083333333333315E-2</v>
       </c>
-      <c r="E165" s="75"/>
+      <c r="E165" s="75" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="96"/>
@@ -4945,63 +4957,95 @@
         <v>0.5</v>
       </c>
       <c r="C166" s="69">
-        <v>0.76041666666666663</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="D166" s="69">
         <f>SUM(C166-B166)</f>
-        <v>0.26041666666666663</v>
-      </c>
-      <c r="E166" s="67"/>
+        <v>0.14583333333333337</v>
+      </c>
+      <c r="E166" s="67" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="73"/>
       <c r="B167" s="76">
         <f>C166</f>
-        <v>0.76041666666666663</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="C167" s="74">
-        <v>0.77083333333333337</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="D167" s="74">
         <f>SUM(C167-B167)</f>
+        <v>8.3333333333333259E-2</v>
+      </c>
+      <c r="E167" s="75" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="67"/>
+      <c r="B168" s="68">
+        <f>C167</f>
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="C168" s="69">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="D168" s="69">
+        <f t="shared" ref="D168" si="17">SUM(C168-B168)</f>
         <v>1.0416666666666741E-2</v>
       </c>
-      <c r="E167" s="75"/>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A168" s="75"/>
-      <c r="B168" s="76">
-        <f>C167</f>
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="C168" s="74">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="D168" s="74">
-        <f t="shared" ref="D168" si="17">SUM(C168-B168)</f>
-        <v>0</v>
-      </c>
-      <c r="E168" s="101"/>
+      <c r="E168" s="102" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="75"/>
-      <c r="B169" s="76"/>
-      <c r="C169" s="74"/>
-      <c r="D169" s="74"/>
+      <c r="B169" s="76">
+        <f t="shared" ref="B169:B171" si="18">C168</f>
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="C169" s="74">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="D169" s="74">
+        <f t="shared" ref="D169:D170" si="19">SUM(C169-B169)</f>
+        <v>2.0833333333333259E-2</v>
+      </c>
       <c r="E169" s="75"/>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A170" s="75"/>
-      <c r="B170" s="76"/>
-      <c r="C170" s="74"/>
-      <c r="D170" s="74"/>
-      <c r="E170" s="75"/>
+      <c r="A170" s="67"/>
+      <c r="B170" s="68">
+        <f t="shared" si="18"/>
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="C170" s="69">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D170" s="69">
+        <f t="shared" si="19"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E170" s="67" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="75"/>
-      <c r="B171" s="76"/>
-      <c r="C171" s="74"/>
-      <c r="D171" s="74"/>
+      <c r="B171" s="76">
+        <f t="shared" si="18"/>
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C171" s="74">
+        <v>0.875</v>
+      </c>
+      <c r="D171" s="74">
+        <f t="shared" ref="D171" si="20">SUM(C171-B171)</f>
+        <v>8.333333333333337E-2</v>
+      </c>
       <c r="E171" s="75"/>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -5039,8 +5083,8 @@
       <c r="B176" s="68"/>
       <c r="C176" s="68"/>
       <c r="D176" s="69">
-        <f>D166</f>
-        <v>0.26041666666666663</v>
+        <f>D166+D168+D170</f>
+        <v>0.18750000000000011</v>
       </c>
       <c r="E176" s="67"/>
     </row>
@@ -5075,7 +5119,7 @@
       <c r="C180" s="93"/>
       <c r="D180" s="94">
         <f>SUM(D165:D174)-(D176+D178)</f>
-        <v>6.2500000000000056E-2</v>
+        <v>0.2395833333333332</v>
       </c>
       <c r="E180" s="93"/>
     </row>

</xml_diff>

<commit_message>
v0.039 Rnd Players w/o duplicates (Fisher-Yates)
</commit_message>
<xml_diff>
--- a/FBM-planning.xlsx
+++ b/FBM-planning.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="130">
   <si>
     <t>M</t>
   </si>
@@ -405,6 +405,9 @@
   </si>
   <si>
     <t>InitPlayers setup team with 10 players works</t>
+  </si>
+  <si>
+    <t>fix, dubletter, init player</t>
   </si>
 </sst>
 </file>
@@ -3037,7 +3040,7 @@
   <dimension ref="A1:G181"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="C172" sqref="C172"/>
+      <selection activeCell="E172" sqref="E172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5046,7 +5049,9 @@
         <f t="shared" ref="D171" si="20">SUM(C171-B171)</f>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E171" s="75"/>
+      <c r="E171" s="75" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="75"/>

</xml_diff>

<commit_message>
v0.040 fix InitPlayers PlayerStats/Value
</commit_message>
<xml_diff>
--- a/FBM-planning.xlsx
+++ b/FBM-planning.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="135">
   <si>
     <t>M</t>
   </si>
@@ -408,6 +408,21 @@
   </si>
   <si>
     <t>fix, dubletter, init player</t>
+  </si>
+  <si>
+    <t>Pluralsight course: Testing xUnit</t>
+  </si>
+  <si>
+    <t>Paus, Verisure m.m.</t>
+  </si>
+  <si>
+    <t>Pluralsight course: Testing xUnit, UserManagerClass, UML</t>
+  </si>
+  <si>
+    <t>Rnd Players</t>
+  </si>
+  <si>
+    <t>Init and List Team Players</t>
   </si>
 </sst>
 </file>
@@ -3037,17 +3052,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G181"/>
+  <dimension ref="A1:G220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="E172" sqref="E172"/>
+    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
+      <selection activeCell="C206" sqref="C206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" customWidth="1"/>
+    <col min="5" max="5" width="61.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -5129,6 +5144,446 @@
       <c r="E180" s="93"/>
     </row>
     <row r="181" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="B183" s="91" t="s">
+        <v>65</v>
+      </c>
+      <c r="C183" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D183" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="E183" s="91" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="73">
+        <v>44643</v>
+      </c>
+      <c r="B184" s="74">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="C184" s="74">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D184" s="74">
+        <f>SUM(C184-B184)</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E184" s="75" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="96"/>
+      <c r="B185" s="68">
+        <f>C184</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C185" s="69">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="D185" s="69">
+        <f>SUM(C185-B185)</f>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="E185" s="67" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="73"/>
+      <c r="B186" s="76">
+        <f>C185</f>
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="C186" s="74">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D186" s="74">
+        <f>SUM(C186-B186)</f>
+        <v>3.8194444444444475E-2</v>
+      </c>
+      <c r="E186" s="75" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="67"/>
+      <c r="B187" s="68">
+        <f>C186</f>
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C187" s="69">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D187" s="69">
+        <f t="shared" ref="D187" si="21">SUM(C187-B187)</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E187" s="102" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="75"/>
+      <c r="B188" s="76">
+        <f t="shared" ref="B188:B194" si="22">C187</f>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C188" s="74">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="D188" s="74">
+        <f t="shared" ref="D188:D190" si="23">SUM(C188-B188)</f>
+        <v>4.8611111111111049E-2</v>
+      </c>
+      <c r="E188" s="75" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="79"/>
+      <c r="B189" s="80">
+        <f t="shared" si="22"/>
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="C189" s="78">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="D189" s="78">
+        <f t="shared" si="23"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E189" s="79" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="75"/>
+      <c r="B190" s="76">
+        <f t="shared" si="22"/>
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="C190" s="74">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="D190" s="74">
+        <f t="shared" si="23"/>
+        <v>5.5555555555555247E-2</v>
+      </c>
+      <c r="E190" s="75" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="67"/>
+      <c r="B191" s="68">
+        <f t="shared" si="22"/>
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="C191" s="69">
+        <v>0.75</v>
+      </c>
+      <c r="D191" s="69">
+        <f t="shared" ref="D191" si="24">SUM(C191-B191)</f>
+        <v>4.1666666666666963E-2</v>
+      </c>
+      <c r="E191" s="67" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="75"/>
+      <c r="B192" s="76">
+        <f t="shared" si="22"/>
+        <v>0.75</v>
+      </c>
+      <c r="C192" s="74">
+        <v>0.79166666666666696</v>
+      </c>
+      <c r="D192" s="74">
+        <f t="shared" ref="D192:D193" si="25">SUM(C192-B192)</f>
+        <v>4.1666666666666963E-2</v>
+      </c>
+      <c r="E192" s="75" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="67"/>
+      <c r="B193" s="68">
+        <f t="shared" si="22"/>
+        <v>0.79166666666666696</v>
+      </c>
+      <c r="C193" s="69">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="D193" s="69">
+        <f t="shared" si="25"/>
+        <v>7.2916666666666408E-2</v>
+      </c>
+      <c r="E193" s="67" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="75"/>
+      <c r="B194" s="76">
+        <f t="shared" si="22"/>
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="C194" s="74">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="D194" s="74">
+        <f t="shared" ref="D194" si="26">SUM(C194-B194)</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E194" s="75" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="75"/>
+      <c r="B195" s="76"/>
+      <c r="C195" s="76"/>
+      <c r="D195" s="74"/>
+      <c r="E195" s="75"/>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="B196" s="68"/>
+      <c r="C196" s="68"/>
+      <c r="D196" s="69">
+        <f>D185+D187+D191+D193</f>
+        <v>0.24305555555555558</v>
+      </c>
+      <c r="E196" s="67"/>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="65"/>
+      <c r="B197" s="66"/>
+      <c r="C197" s="66"/>
+      <c r="D197" s="64"/>
+      <c r="E197" s="65"/>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="79" t="s">
+        <v>85</v>
+      </c>
+      <c r="B198" s="80"/>
+      <c r="C198" s="80"/>
+      <c r="D198" s="78">
+        <f>D189</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E198" s="79"/>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="65"/>
+      <c r="B199" s="66"/>
+      <c r="C199" s="66"/>
+      <c r="D199" s="64"/>
+      <c r="E199" s="65"/>
+    </row>
+    <row r="200" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A200" s="93" t="s">
+        <v>86</v>
+      </c>
+      <c r="B200" s="93"/>
+      <c r="C200" s="93"/>
+      <c r="D200" s="94">
+        <f>SUM(D184:D194)-(D196+D198)</f>
+        <v>0.24652777777777779</v>
+      </c>
+      <c r="E200" s="93"/>
+    </row>
+    <row r="201" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="B203" s="91" t="s">
+        <v>65</v>
+      </c>
+      <c r="C203" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D203" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="E203" s="91" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="73">
+        <v>44644</v>
+      </c>
+      <c r="B204" s="74">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C204" s="74">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D204" s="74">
+        <f>SUM(C204-B204)</f>
+        <v>0.14583333333333337</v>
+      </c>
+      <c r="E204" s="75"/>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="96"/>
+      <c r="B205" s="68">
+        <f>C204</f>
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C205" s="69">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D205" s="69">
+        <f>SUM(C205-B205)</f>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="E205" s="67" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="73"/>
+      <c r="B206" s="76">
+        <f>C205</f>
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C206" s="74">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D206" s="74">
+        <f>SUM(C206-B206)</f>
+        <v>0.25</v>
+      </c>
+      <c r="E206" s="75"/>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="75"/>
+      <c r="B207" s="76">
+        <f>C206</f>
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C207" s="74">
+        <v>0.875</v>
+      </c>
+      <c r="D207" s="74">
+        <f t="shared" ref="D207" si="27">SUM(C207-B207)</f>
+        <v>0.10416666666666663</v>
+      </c>
+      <c r="E207" s="101"/>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="75"/>
+      <c r="B208" s="76"/>
+      <c r="C208" s="74"/>
+      <c r="D208" s="74"/>
+      <c r="E208" s="75"/>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="75"/>
+      <c r="B209" s="76"/>
+      <c r="C209" s="74"/>
+      <c r="D209" s="74"/>
+      <c r="E209" s="75"/>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="75"/>
+      <c r="B210" s="76"/>
+      <c r="C210" s="74"/>
+      <c r="D210" s="74"/>
+      <c r="E210" s="75"/>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="75"/>
+      <c r="B211" s="76"/>
+      <c r="C211" s="74"/>
+      <c r="D211" s="74"/>
+      <c r="E211" s="75"/>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" s="75"/>
+      <c r="B212" s="76"/>
+      <c r="C212" s="74"/>
+      <c r="D212" s="74"/>
+      <c r="E212" s="75"/>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="75"/>
+      <c r="B213" s="76"/>
+      <c r="C213" s="74"/>
+      <c r="D213" s="74"/>
+      <c r="E213" s="75"/>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="75"/>
+      <c r="B214" s="76"/>
+      <c r="C214" s="76"/>
+      <c r="D214" s="74"/>
+      <c r="E214" s="75"/>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="B215" s="68"/>
+      <c r="C215" s="68"/>
+      <c r="D215" s="69">
+        <f>D205</f>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="E215" s="67"/>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="65"/>
+      <c r="B216" s="66"/>
+      <c r="C216" s="66"/>
+      <c r="D216" s="64"/>
+      <c r="E216" s="65"/>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="79" t="s">
+        <v>85</v>
+      </c>
+      <c r="B217" s="80"/>
+      <c r="C217" s="80"/>
+      <c r="D217" s="78"/>
+      <c r="E217" s="79"/>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="65"/>
+      <c r="B218" s="66"/>
+      <c r="C218" s="66"/>
+      <c r="D218" s="64"/>
+      <c r="E218" s="65"/>
+    </row>
+    <row r="219" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A219" s="93" t="s">
+        <v>86</v>
+      </c>
+      <c r="B219" s="93"/>
+      <c r="C219" s="93"/>
+      <c r="D219" s="94">
+        <f>SUM(D204:D213)-(D215+D217)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E219" s="93"/>
+    </row>
+    <row r="220" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
v0.040 Fix InitPlayers Stats+Value, ListPlayers
</commit_message>
<xml_diff>
--- a/FBM-planning.xlsx
+++ b/FBM-planning.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="139">
   <si>
     <t>M</t>
   </si>
@@ -423,6 +423,18 @@
   </si>
   <si>
     <t>Init and List Team Players</t>
+  </si>
+  <si>
+    <t>Presentationsmaterial; Powerpoint, Flowchart, UML mm.</t>
+  </si>
+  <si>
+    <t>Curonova Möte Teams, Grupp</t>
+  </si>
+  <si>
+    <t>Curonova Möte Telefon, Handledare</t>
+  </si>
+  <si>
+    <t>Fix InitPlayer Stats + Value</t>
   </si>
 </sst>
 </file>
@@ -742,7 +754,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -862,6 +874,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3054,8 +3067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
-      <selection activeCell="C206" sqref="C206"/>
+    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="E209" sqref="E209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5425,94 +5438,138 @@
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A204" s="73">
+      <c r="A204" s="81">
         <v>44644</v>
       </c>
-      <c r="B204" s="74">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C204" s="74">
+      <c r="B204" s="82">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C204" s="82">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D204" s="82">
+        <f>SUM(C204-B204)</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E204" s="83" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="81"/>
+      <c r="B205" s="84">
+        <f>C204</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C205" s="82">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D205" s="82">
+        <f>SUM(C205-B205)</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E205" s="103" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="96"/>
+      <c r="B206" s="68">
+        <f>C205</f>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C206" s="69">
         <v>0.47916666666666669</v>
       </c>
-      <c r="D204" s="74">
-        <f>SUM(C204-B204)</f>
-        <v>0.14583333333333337</v>
-      </c>
-      <c r="E204" s="75"/>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A205" s="96"/>
-      <c r="B205" s="68">
-        <f>C204</f>
+      <c r="D206" s="69">
+        <f>SUM(C206-B206)</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E206" s="92" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="83"/>
+      <c r="B207" s="84">
+        <f>C206</f>
         <v>0.47916666666666669</v>
       </c>
-      <c r="C205" s="69">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="D205" s="69">
-        <f>SUM(C205-B205)</f>
-        <v>4.1666666666666685E-2</v>
-      </c>
-      <c r="E205" s="67" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A206" s="73"/>
-      <c r="B206" s="76">
-        <f>C205</f>
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="C206" s="74">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="D206" s="74">
-        <f>SUM(C206-B206)</f>
-        <v>0.25</v>
-      </c>
-      <c r="E206" s="75"/>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A207" s="75"/>
-      <c r="B207" s="76">
-        <f>C206</f>
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="C207" s="74">
-        <v>0.875</v>
-      </c>
-      <c r="D207" s="74">
+      <c r="C207" s="82">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D207" s="82">
         <f t="shared" ref="D207" si="27">SUM(C207-B207)</f>
-        <v>0.10416666666666663</v>
-      </c>
-      <c r="E207" s="101"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E207" s="103" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="75"/>
-      <c r="B208" s="76"/>
-      <c r="C208" s="74"/>
-      <c r="D208" s="74"/>
-      <c r="E208" s="75"/>
+      <c r="B208" s="76">
+        <f t="shared" ref="B208:B211" si="28">C207</f>
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="C208" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D208" s="74">
+        <f t="shared" ref="D208:D209" si="29">SUM(C208-B208)</f>
+        <v>5.2083333333333315E-2</v>
+      </c>
+      <c r="E208" s="75" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="75"/>
-      <c r="B209" s="76"/>
-      <c r="C209" s="74"/>
-      <c r="D209" s="74"/>
-      <c r="E209" s="75"/>
+      <c r="B209" s="76">
+        <f t="shared" si="28"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C209" s="74">
+        <v>0.57291666666666696</v>
+      </c>
+      <c r="D209" s="74">
+        <f t="shared" si="29"/>
+        <v>3.1250000000000333E-2</v>
+      </c>
+      <c r="E209" s="99" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="75"/>
-      <c r="B210" s="76"/>
-      <c r="C210" s="74"/>
-      <c r="D210" s="74"/>
-      <c r="E210" s="75"/>
+      <c r="B210" s="76">
+        <f t="shared" si="28"/>
+        <v>0.57291666666666696</v>
+      </c>
+      <c r="C210" s="74">
+        <v>0.61458333333333404</v>
+      </c>
+      <c r="D210" s="74">
+        <f t="shared" ref="D210:D211" si="30">SUM(C210-B210)</f>
+        <v>4.1666666666667074E-2</v>
+      </c>
+      <c r="E210" s="75" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="75"/>
-      <c r="B211" s="76"/>
-      <c r="C211" s="74"/>
-      <c r="D211" s="74"/>
+      <c r="B211" s="76">
+        <f t="shared" si="28"/>
+        <v>0.61458333333333404</v>
+      </c>
+      <c r="C211" s="74">
+        <v>0.65625</v>
+      </c>
+      <c r="D211" s="74">
+        <f t="shared" si="30"/>
+        <v>4.1666666666665964E-2</v>
+      </c>
       <c r="E211" s="75"/>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -5543,8 +5600,8 @@
       <c r="B215" s="68"/>
       <c r="C215" s="68"/>
       <c r="D215" s="69">
-        <f>D205</f>
-        <v>4.1666666666666685E-2</v>
+        <f>D206</f>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="E215" s="67"/>
     </row>
@@ -5579,7 +5636,7 @@
       <c r="C219" s="93"/>
       <c r="D219" s="94">
         <f>SUM(D204:D213)-(D215+D217)</f>
-        <v>0.5</v>
+        <v>0.23958333333333331</v>
       </c>
       <c r="E219" s="93"/>
     </row>

</xml_diff>

<commit_message>
v0.043 Fix PlayerUpdate PlayerRepository
</commit_message>
<xml_diff>
--- a/FBM-planning.xlsx
+++ b/FBM-planning.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="144">
   <si>
     <t>M</t>
   </si>
@@ -444,6 +444,12 @@
   </si>
   <si>
     <t>PlayerSubstitution</t>
+  </si>
+  <si>
+    <t>Navigation and Selection of Players in List Players</t>
+  </si>
+  <si>
+    <t>Jobbsök Sogeti m.m.</t>
   </si>
 </sst>
 </file>
@@ -763,7 +769,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -891,6 +897,8 @@
     <xf numFmtId="165" fontId="0" fillId="21" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="18" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="18" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="20" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="20" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3081,10 +3089,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G220"/>
+  <dimension ref="A1:G239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
-      <selection activeCell="D219" sqref="D219"/>
+    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="E225" sqref="E225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5682,6 +5690,233 @@
       <c r="E219" s="93"/>
     </row>
     <row r="220" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="B222" s="91" t="s">
+        <v>65</v>
+      </c>
+      <c r="C222" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D222" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="E222" s="91" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="73">
+        <v>44645</v>
+      </c>
+      <c r="B223" s="74">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="C223" s="74">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D223" s="74">
+        <f>SUM(C223-B223)</f>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="E223" s="75" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="81"/>
+      <c r="B224" s="104">
+        <f>C223</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C224" s="105">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D224" s="105">
+        <f>SUM(C224-B224)</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E224" s="103" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" s="96"/>
+      <c r="B225" s="68">
+        <f>C224</f>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C225" s="69">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D225" s="69">
+        <f>SUM(C225-B225)</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E225" s="67"/>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" s="101"/>
+      <c r="B226" s="111">
+        <f>C225</f>
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C226" s="112">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D226" s="112">
+        <f t="shared" ref="D226:D232" si="32">SUM(C226-B226)</f>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E226" s="77"/>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="75"/>
+      <c r="B227" s="76">
+        <f t="shared" ref="B227:B232" si="33">C226</f>
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="C227" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D227" s="74">
+        <f t="shared" si="32"/>
+        <v>5.2083333333333315E-2</v>
+      </c>
+      <c r="E227" s="75"/>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="75"/>
+      <c r="B228" s="76">
+        <f t="shared" si="33"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C228" s="74">
+        <v>0.59375</v>
+      </c>
+      <c r="D228" s="74">
+        <f t="shared" si="32"/>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="E228" s="75"/>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="101"/>
+      <c r="B229" s="111">
+        <f t="shared" si="33"/>
+        <v>0.59375</v>
+      </c>
+      <c r="C229" s="112">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="D229" s="112">
+        <f t="shared" si="32"/>
+        <v>5.902777777777779E-2</v>
+      </c>
+      <c r="E229" s="101"/>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="75"/>
+      <c r="B230" s="76">
+        <f t="shared" si="33"/>
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="C230" s="74">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D230" s="74">
+        <f t="shared" si="32"/>
+        <v>5.555555555555558E-2</v>
+      </c>
+      <c r="E230" s="75"/>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" s="75"/>
+      <c r="B231" s="76">
+        <f t="shared" si="33"/>
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C231" s="74">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D231" s="74">
+        <f t="shared" si="32"/>
+        <v>0.125</v>
+      </c>
+      <c r="E231" s="75"/>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" s="75"/>
+      <c r="B232" s="76">
+        <f t="shared" si="33"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C232" s="74">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D232" s="74">
+        <f t="shared" si="32"/>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="E232" s="75"/>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="75"/>
+      <c r="B233" s="76"/>
+      <c r="C233" s="76"/>
+      <c r="D233" s="74"/>
+      <c r="E233" s="75"/>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="B234" s="68"/>
+      <c r="C234" s="68"/>
+      <c r="D234" s="69">
+        <f>D225</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E234" s="67"/>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" s="65"/>
+      <c r="B235" s="66"/>
+      <c r="C235" s="66"/>
+      <c r="D235" s="64"/>
+      <c r="E235" s="65"/>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" s="79" t="s">
+        <v>85</v>
+      </c>
+      <c r="B236" s="80"/>
+      <c r="C236" s="80"/>
+      <c r="D236" s="78"/>
+      <c r="E236" s="79"/>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" s="65"/>
+      <c r="B237" s="66"/>
+      <c r="C237" s="66"/>
+      <c r="D237" s="64"/>
+      <c r="E237" s="65"/>
+    </row>
+    <row r="238" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A238" s="93" t="s">
+        <v>86</v>
+      </c>
+      <c r="B238" s="93"/>
+      <c r="C238" s="93"/>
+      <c r="D238" s="94">
+        <f>SUM(D223:D232)-(D234+D236)</f>
+        <v>0.46874999999999994</v>
+      </c>
+      <c r="E238" s="93"/>
+    </row>
+    <row r="239" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>